<commit_message>
Se arreglan problemas de compatabilidad con R 4.0.0
</commit_message>
<xml_diff>
--- a/data/intermediate/001_Herramienta_Limpieza_Manual.xlsx
+++ b/data/intermediate/001_Herramienta_Limpieza_Manual.xlsx
@@ -1,30 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documentos\Estudio_Documentos\Trabajos\UAS-FNE-2\61_Regionalizacion\FRE_AnalisisEstadistico\data\intermediate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\OneDrive\Documents\Trabajos\UAS-FNE-2\61_Regionalizacion\FRE_AnalisisEstadistico\data\intermediate\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CA66F7-FC93-4377-966C-247C1F6152CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" tabRatio="456"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respuestas de formulario 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Daniel S. Parra G.</author>
   </authors>
   <commentList>
-    <comment ref="BG2" authorId="0" shapeId="0">
+    <comment ref="BG2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -48,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT7" authorId="0" shapeId="0">
+    <comment ref="AT7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -72,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AY10" authorId="0" shapeId="0">
+    <comment ref="AY10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -101,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="981">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2104" uniqueCount="1228">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -3139,11 +3151,790 @@
   <si>
     <t>San Jose de Cúcuta</t>
   </si>
+  <si>
+    <t>Juan Pablo Arias</t>
+  </si>
+  <si>
+    <t>Leonor del Carmen Valoyes Murillo</t>
+  </si>
+  <si>
+    <t>San José del Guaviare</t>
+  </si>
+  <si>
+    <t>Calle 7 No. 23 - 51</t>
+  </si>
+  <si>
+    <t>ssdgsaludambiental12@gmail.com</t>
+  </si>
+  <si>
+    <t>Decreto 216 de 2016</t>
+  </si>
+  <si>
+    <t>Heidy Tatiana Parra Penagos</t>
+  </si>
+  <si>
+    <t>Heydeer Yovanny Palacio Salazar</t>
+  </si>
+  <si>
+    <t>Gregorio Figueroa Cruz</t>
+  </si>
+  <si>
+    <t>Técnico Área en salud</t>
+  </si>
+  <si>
+    <t>Auxiliar en salud</t>
+  </si>
+  <si>
+    <t>Ingeniero Químico</t>
+  </si>
+  <si>
+    <t>Elizabeth Poveda Jimenez</t>
+  </si>
+  <si>
+    <t>Fidelina Rojas</t>
+  </si>
+  <si>
+    <t>Julian Sarmiento Pardo</t>
+  </si>
+  <si>
+    <t>Abogado</t>
+  </si>
+  <si>
+    <t>Personal del FRE proyecta la creación de la necesidad y se hacen estudios de compra, donde se incluyen las solicitudes de cotización a diferentes litografías. La secretaria de salud aprueba los documentos y al mismo tiempo, solicitan CDP por parte de la Secretaria de Salud del Guaviare. Luego, la documentación se envía a la secretaria de hacienda departamental del Guaviare. Posteriormente, la documentación pasa por diferentes dependencias de la Gobernación de Guaviare, como el área jurídica departamental, área financiera departamental y el área encargada del plan de compras departamental. Los documentos retornan a la secretaria de salud con el visto bueno de la Gobernación del Guaviare, para ser enviados nuevamente al área jurídica de la gobernación, quienes son los encargados de la parte contractual.</t>
+  </si>
+  <si>
+    <t>Se lleva a cabo de acuerdo al consumo histórico mensual de recetarios oficiales y se incrementan entre 5 y 20 talonarios para evitar un margen ajustado de recetarios oficiales en el departamento.</t>
+  </si>
+  <si>
+    <t>Creación de la necesidad y estudios de compra: 3 días. 
+Aprobación de la Secretaria de salud: 1 día.
+Aprobación por parte de todas las áreas de la Gobernación de Guaviare: 7 días.
+Publicación de la convocatoria 1 día.
+Recepción de los recetarios oficiales: 2 días.</t>
+  </si>
+  <si>
+    <t>La institución prestadora de salud inicia la solicitud con la radicación de un oficio de manera presencial en la Gobernación de Guaviare. Esta solicitud también la realizan vía WhatsApp con destino al personal del FRE para aligerar el proceso con el personal encargado de la distribución de los recetarios oficiales. El oficio llega a la Secretaria de Salud del Guaviare, específicamente al área ambiental, donde es recibido por el personal del FRE. La Auxiliar en salud es la encargada de la venta y distribución de los recetarios oficiales. Ella se comunica con la institución para mencionar el costo de los recetarios solicitados y el número de cuenta para hacer la consignación bancaria. Una vez se cumpla lo anterior, se acercan a la Secretaria de Salud del Guaviare con el comprobante de la consignación y se hace entrega de los talonarios.</t>
+  </si>
+  <si>
+    <t>Nombre de persona, Documento de identificación, Códigos seriales de recetarios, Otros</t>
+  </si>
+  <si>
+    <t>Códigos seriales de recetarios que devuelven</t>
+  </si>
+  <si>
+    <t>No lo tienen</t>
+  </si>
+  <si>
+    <t>Facilitarían los procesos internos y con los pacientes. Además, se lograría la estandarización de los niveles de seguridad que deben tener los recetarios oficiales a nivel nacional. Sin embargo, se contemplan problemas de conectividad a internet y se compara el manejo con la herramienta tecnológica actual “Mipres”, cuya plataforma presenta inconvenientes en el territorio.
+FRE Guaviare no encuentra inconvenientes en las ganancias originadas por la venta de los recetarios oficiales, ya que el precio de compra es muy similar al precio de venta.</t>
+  </si>
+  <si>
+    <t>Verficación de base de ventas, Verificación de recambios, Visitas a institciones/clientes, Otro</t>
+  </si>
+  <si>
+    <t>Listado del personal médico autorizado para la prescripción de MME</t>
+  </si>
+  <si>
+    <t>Siempre se remiten a la IPS para confirmar la información de los recetarios oficiales. Se verifican códigos de los recetarios oficiales distribuidos a la IPS. Cuando se pierde algún recetario oficial, la institución debe hacer la respectiva denuncia con las autoridades competentes poder aceptar la pérdida del recetario oficial. Se pone en alerta el número del talonario del recetario extraviado. La información se consolida en la base de datos de venta y distribución de recetarios oficiales.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La Auxiliar en salud encargada de la gestión de los recetarios oficiales, revisa todos los días las existencias de estos recetarios. Ella conoce el consumo aproximado de cada institución autorizada. En caso de tener un nivel muy bajo de existencias, comienza las cotizaciones para la proyección de compra. </t>
+  </si>
+  <si>
+    <t>Los recetarios oficiales usados deben ser regresados al FRE cada vez que la institución realice la siguiente compra de recetarios oficiales en blanco. El personal del FRE verifica que no falte ninguna prescripción por cada talonario. En caso de faltar, debe estar justificado con la respectiva denuncia y mencionar el código del recetario extraviado. FRE Guaviare pone en alerta en todo el territorio el código del recetario extraviado y el número del talonario.</t>
+  </si>
+  <si>
+    <t>Microletras / microtexto, Sellos/Escudos, Codificación, Otro</t>
+  </si>
+  <si>
+    <t>Código de seguridad inmerso en la codificación.</t>
+  </si>
+  <si>
+    <t>Es un proceso llevado a cabo por la Auxiliar en salud, cada vez que se va a vender nuevos recetarios oficiales. Ella verifica que se encuentren todas las hojas (prescripciones) del talonario, que no presenten inconsistencias en el diligenciamiento y que se haya dispensado el medicamento. Cuando se encuentran irregularidades, se levanta una medida sanitaria.</t>
+  </si>
+  <si>
+    <t>La revisión y consolidación es realizada por 1 persona y tarda aproximadamente 1 día.</t>
+  </si>
+  <si>
+    <t>Gabinete con llave, Almaceamiento en oficina privada</t>
+  </si>
+  <si>
+    <t>La empresa encargada de la disposición final de productos y recetarios oficiales, realiza esta actividad.</t>
+  </si>
+  <si>
+    <t>Codificación, Nombre prescriptor, Documento de identificación, Nombre del paciente, Cantidad total</t>
+  </si>
+  <si>
+    <t>Atención presencial en el FRE, Teléfono, Correo electrónico, Correspondencia</t>
+  </si>
+  <si>
+    <t>La Auxiliar en salud, el ingeniero químico y la regente en farmacia llevan a cabo este proceso. Se considera el consumo mensual de MME, el consumo histórico desde la creación del FRE y la existencia actual de MME. La base de datos empleada para este proceso se va alimentando a cada instante, por las salidas y entradas de MME. Personal del FRE, contempla un porcentaje demás para no quedar con un margen tan apretado de MME. Muchas veces, la proyección de compra debe ser modificado por disponibilidad de recursos de la Gobernación de Guaviare.</t>
+  </si>
+  <si>
+    <t>No conocen este tiempo</t>
+  </si>
+  <si>
+    <t>Personal del FRE estaba acostumbrado al proceso realizado anteriormente. Al principio de la implementación de la plataforma Colombia Compra Eficiente estaban en desacuerdo por que el personal que maneja la plataforma no sabía cómo usarla. Actualmente, no tienen opiniones por que el personal del FRE no maneja esta plataforma.</t>
+  </si>
+  <si>
+    <t>Inicialmente, se verifican que las cajas vengan en excelente estado, sin adulteraciones. Luego, se verifica el interior de cada caja y el estado de los MME. El personal del FRE, verifica los datos (lote y fecha de vencimiento) de la factura que envía el FNE y la información proveniente de la caja. Finalmente se diligencia el acta de recepción.</t>
+  </si>
+  <si>
+    <t>Se toma la evidencia fotográfica de los productos y se deja nota en el acta de recepción. Se notifica inmediatamente al FNE y quedan pendientes de la reposición de las existencias.</t>
+  </si>
+  <si>
+    <t>Gabinete con llave simple, Gabinete hecho en un material resistente, Acceso de seguridad restringido a cierto personal, Inventario físico diario, Disponibilidad local de protección policial</t>
+  </si>
+  <si>
+    <t>Tienen una góndola exclusiva y destinada para el almacenamiento de medicamentos LASA y alto riesgo.</t>
+  </si>
+  <si>
+    <t>El FNE siempre responde y efectúa la devolución de los productos con averías. Personal del FRE, reconoce que cuando sucede esto es por una falla en el proceso de embalaje y no es responsabilidad de la empresa transportadora.</t>
+  </si>
+  <si>
+    <t>En la central de medicamentos se verifican existencias de los MME y esta información se compara con el contenido del libro en físico de inventario. Cada 20 días llevan a cabo la verificación exhaustiva de existencias y fechas de vencimiento.</t>
+  </si>
+  <si>
+    <t>Rojo: menor a 3 meses
+Amarillo: 3 meses - 6 meses
+Verde: mayor a 6 meses</t>
+  </si>
+  <si>
+    <t>Tienen suficiente espacio, la góndola de MME está ocupada el 20% solamente.</t>
+  </si>
+  <si>
+    <t>Ningún costo</t>
+  </si>
+  <si>
+    <t>En 2018, Hidromorfona (240 unidades – 12 cajas).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El proceso inicio con un oficio firmado por el representante legal de la IPS, dirigida a la Secretaria de Salud del Guaviare. Actualmente, este proceso se agiliza por medio del WhatsApp entre el solicitante y la Auxiliar en salud del FRE. Personal del FRE Guaviare, verifica la disponibilidad de existencias de medicamentos. Se envía la factura para que la IPS consigne el valor de los MME. </t>
+  </si>
+  <si>
+    <t>No reciben devoluciones.</t>
+  </si>
+  <si>
+    <t>Si han recibido quejas, por razones de la pandemia y problemas con el transporte. FRE recomienda a las IPS hacer compra directa con el FNE.</t>
+  </si>
+  <si>
+    <t>Los pacientes llevan el recetario oficial y se verifica que este bien diligenciado y el tiempo límite de dispensación. Se le informa al paciente el número de cuenta bancaria y el valor que deben consignar para el medicamento. Los pacientes que ya conocen a la Auxiliar en salud del FRE, agilizan el proceso vía WhatsApp. En muy pocos casos, los pacientes que presentan dificultades para realizar la consignación, son asistidos por la Auxiliar en salud y ella misma hace la consignación bancaria con el dinero del paciente.</t>
+  </si>
+  <si>
+    <t>No se han encontrado irregularidades durante la venta y dispensación en pacientes. Únicamente recetarios diligenciados de manera incompleta, se procedió a informar a cada médico prescriptor que debía hacer el diligenciamiento completo.</t>
+  </si>
+  <si>
+    <t>Se llama al otro FRE y ellos escalan la pregunta con la IPS de su territorio. Se valida la información de la institución y que el médico prescriptor este habilitado. Luego, buscan un médico del territorio de Guaviare para reformular los medicamentos en un recetario oficial del departamento de Guaviare. Se anexa la copia del recetario oficial inicial.</t>
+  </si>
+  <si>
+    <t>No han tenido estos casos.</t>
+  </si>
+  <si>
+    <t>Hacen corte al último día del mes, verifican el libro de inventarios y las facturas tanto de las ventas a pacientes como las ventas a las IPS. Se diligencia el Excel.</t>
+  </si>
+  <si>
+    <t>Documentos físico, Hoja de cálculo no estandarizada</t>
+  </si>
+  <si>
+    <t>Se maneja un archivo físico y archivo virtual para los informes recibidos por el correo. Cada uno está ordenado por carpetas por IPS y por mes</t>
+  </si>
+  <si>
+    <t>2 personas y se destinan 8 horas para la consolidación.</t>
+  </si>
+  <si>
+    <t>Personal del FRE hace una lista de chequeo donde están todas las IPS habilitadas. Se revisa el correo electrónico y se verifica que la IPS envió el archivo.</t>
+  </si>
+  <si>
+    <t>Amonestación, Multa</t>
+  </si>
+  <si>
+    <t>Si tienen un consolidado de las IPS y su complejidad.</t>
+  </si>
+  <si>
+    <t>Oficialmente no tienen POEs. Actualmente existe un borrador que está en proceso de revisión jurídica. Personal del FRE no quiere mostrar este documento porque no es oficial.</t>
+  </si>
+  <si>
+    <t>Juan David Apraez</t>
+  </si>
+  <si>
+    <t>Carrera 4 #8-26, barrio Jose Maria Hernandez</t>
+  </si>
+  <si>
+    <t>fvputumayo@gmail.com; gestionssd@gmail.com; medicamentosputumayo@gmail.com; salud@putumayo.gov.co; saludpublica@putumayo.gov.co</t>
+  </si>
+  <si>
+    <t>Resolución 1696</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mónica Guerrero Rendon </t>
+  </si>
+  <si>
+    <t>Elva Marina Rosero Ordoñez</t>
+  </si>
+  <si>
+    <t>Aurora Velandia</t>
+  </si>
+  <si>
+    <t>Nora Gelpud</t>
+  </si>
+  <si>
+    <t>El FRE no se encarga del proceso de contratación. Únicamente se encargan de pasar al grupo jurídico la necesidad y la solicitud de los recursos. Ellos se encargan de la parte contractual.</t>
+  </si>
+  <si>
+    <t>Se realiza mediante el promedio histórico de consumo del departamento dado en el sistema PCT</t>
+  </si>
+  <si>
+    <t>Tiempo variante, el FRE Putumayo lleva sin concretar compra de recetarios oficiales desde noviembre del año 2020.</t>
+  </si>
+  <si>
+    <t>Resolución 2226 de 19 de diciembre de 2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Se realiza la cotización de recetarios oficiales
+-Se hace estudio de disponibilidad de recetarios contra los que el establecimiento requiere
+- La institución consigna en la cuenta bancaria del FRE
+- Allegan soportes de pago presencial o a través de envíos de la transportadora que contrata la gobernación.
+</t>
+  </si>
+  <si>
+    <t>Sistema PCT</t>
+  </si>
+  <si>
+    <t>Tipo de persona (comprador), Documento de identificación, Unidades compradas, Códigos seriales de recetarios</t>
+  </si>
+  <si>
+    <t>No se tiene plan de contingencia escrito, sin embargo, ante la no disponibilidad de recetarios oficiales como se encuentra el FRE en este momento, se procede a autorizar las fórmulas institucionales que están bajo jurisdicción del departamento.</t>
+  </si>
+  <si>
+    <t>El uso de recetario oficial en físico es algo obsoleto, hoy en día con todas las herramientas tecnológicas se puede usar un recetario electrónico adaptado a un software para mejorar el control sobre las prescripciones, ya que usualmente entender la letra de los médicos es complejo, no se diligencian todos los campos, no se firman en ocasiones los recetarios, a diferencia que si se tuviera una herramienta tecnológica si no se completan todos los espacios no se tienen estos problemas.</t>
+  </si>
+  <si>
+    <t>No se han presentado casos de posibles fraudes o desvíos. Solo se distribuye a instituciones inscritas de forma personal quienes la entidad delegue o por correo certificado.</t>
+  </si>
+  <si>
+    <t>No se realiza la actividad de control de existencias y saldos de recetarios oficiales en el momento</t>
+  </si>
+  <si>
+    <t>Marcas de agua, Codificación</t>
+  </si>
+  <si>
+    <t>-Se allegan copia de recetario con los informes mensuales. 
+-Revisión de algunos de los recetarios. 
+-Se hace promedio de cuantas salieron, se saca una muestra y se hace la verificación del correcto diligenciamiento. 
+-Archivo por un año porque ocupan bastante espacio además que, por las condiciones ambientales del departamento de Putumayo, la humedad tiende a degradar los recetarios.</t>
+  </si>
+  <si>
+    <t>Una regente de farmacia se encarga del proceso durante los primeros 10 días del mes</t>
+  </si>
+  <si>
+    <t>La secretaria anualmente hace contrato con una empresa recolectora de residuos. El FRE tanto para MME como para recetarios oficiales, se hace una previa de desactivación a los MME y para los recetarios se rasgan para que no puedan ser utilizados nuevamente. Se levanta un acta de destrucción donde se relacionan los productos destruidos, firma la oficina de control de medicamentos, jefe del grupo de salud pública, el área ambiental y el personal de la empresa recolectora. Ambiental se queda con los recibos que se generan para la ejecución del contrato.</t>
+  </si>
+  <si>
+    <t>PCT</t>
+  </si>
+  <si>
+    <t>Mala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se tienen 90 millones de pesos represados porque no saben cómo liquidar los contratos que tienen pendientes, ni los funcionarios del FRE ni jurídica. Dicho rubro se quiere destinar para actualizar equipos de cómputo, así como artículos de la oficina como escritorios y asientos.
+Los informes consolidados en Microsoft Excel se buscan ser migrada a la nube para que las entidades inscritas ante el FRE envíen el reporte directamente a los servidores y así obtener la información del departamento con mayor rapidez.
+La conexión en general en el departamento no es buena, en el momento de hacer la reunión el encargado del FRE atiende desde su teléfono móvil personal.
+El FRE cuenta con dos computadores, sin embargo, en la oficina está el grupo de IVC también con 2 computadores y almacén departamental con otros 2 equipos de cómputo.
+El FRE Huila ha apoyado y dado recomendación al FRE Putumayo en algunos procesos en los que no se tiene claridad. </t>
+  </si>
+  <si>
+    <t>El sistema PCT de acuerdo con las salidas históricas mensuales del FRE, con ello se establece las cantidades a pedir. Luego de ello se revisan los recursos disponibles para realizar el proceso de compra ya que no siempre se cuenta con el rubro necesario para la compra necesaria. El último rubro para compra de MME fue de 25 millones de pesos. Se presentó una demora con Colombia compra eficiente porque se tuvo que cambiar ordenador del gasto y se presentó un problema con un archivo que daba error en la plataforma lo que tardó 5 días en resolverse.
+-	Se otorga el rubro
+-	Se pasa el plan anual
+-	Solicitud de CDP
+-	Luego con la factura de Colombia compra eficiente se expide el RP
+-	Se envían documentos al correo de FNE</t>
+  </si>
+  <si>
+    <t>1-15</t>
+  </si>
+  <si>
+    <t>Pese a que tuvieron algunos problemas con la compra de MME a través de la plataforma el encargado del FRE manifiesta que es eficiente y con la ayuda del soporte técnico de la plataforma pudo concretar la orden de compra.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Los productos llegan a las instalaciones de la secretaria de salud departamental
+- se recibe al transportador y se constata la factura y guía de factura
+- Los medicamentos ingresan al deposito
+- En los mesones se realiza el proceso de recepción administrativa y técnica
+- Se ingresa al sistema de la gobernación los productos recibidos 
+- Se procede a realizar el almacenamiento de los medicamentos. </t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>No se han presentado casos de productos no conformes o averiados. De llegar a pasar se procedería a notificar mediante llamada telefónica con el doctor Pedro con registro fotográfico para la reposición. Si no hubiese cabida a reposición se entregaría a la empresa recolectora para su destrucción.</t>
+  </si>
+  <si>
+    <t>Gabinete con llave simple, Acceso de seguridad restringido a cierto personal, Almacenamiento en oficina privada, Inventario físico diario</t>
+  </si>
+  <si>
+    <t>No se cuentan con medicamentos LASA ni de alto riesgo en la bodega donde están los MME por lo que no se requiere estrategias para el manejo de este tipo de medicamentos.</t>
+  </si>
+  <si>
+    <t>Medicamentos de Salud Pública, Vac</t>
+  </si>
+  <si>
+    <t>El encargado del FRE no ha concebido una opinión concreta del trasportador ya que su vinculación al ente territorial se dio posterior a la última compra de MME.</t>
+  </si>
+  <si>
+    <t>Se hace revisión en el sistema PCT, sin embargo, el funcionario del FRE manifiesta que así se lleve un adecuado control del inventario si no se esta abasteciendo continua y efectivamente el stock de MME el proceso de control de existencias y fechas de vencimiento no es del todo eficiente.</t>
+  </si>
+  <si>
+    <t>No se tiene un estimado del número de medicamentos máximo que pudieran almacenar en el almacén</t>
+  </si>
+  <si>
+    <t>No hay costo alguno en concepto de almacenamiento por parte del FRE</t>
+  </si>
+  <si>
+    <t>Fenobarbital 40 mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Se hace cotización
+- Se hace estudio y aprobación de las cantidades solicitadas
+- se realiza consignación a la cuenta bancaria del FRE
+- Allegan soportes de pago y documentos necesarios para la compra
+- Se autoriza y despacha la orden de compra de MME.
+</t>
+  </si>
+  <si>
+    <t>No se ha dado el caso de devoluciones por parte de las instituciones. Si llegado el caso se despachara el producto en buen estado y cumpliendo especificaciones, pero en el transcurso del transporte a la institución se averió el FRE no se hace responsable.</t>
+  </si>
+  <si>
+    <t>No se han dado quejas formales, pero si se han dado casos en los que por falta de disponibilidad del FRE se autoriza realizar compra directa al FNE.</t>
+  </si>
+  <si>
+    <t>No se vende a pacientes particulares</t>
+  </si>
+  <si>
+    <t>No se ha dado el caso ya que no se dispensa directamente a particulares</t>
+  </si>
+  <si>
+    <t>No se ha dado el caso, pero dado que llegase a pasar se recomendaría transcribir el recetario a uno oficial del departamento de Putumayo</t>
+  </si>
+  <si>
+    <t>No se ha dado el caso, pero dado que llegase a pasar se recomendaría transcribir la formula a un recetario oficial del departamento de Putumayo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las instituciones inscritas envían sus informes de en los 10 primeros días del mes junto con las copias de los recetarios oficiales. Esto se envía en físico y por vía electrónica. Posterior a ello una regente de farmacia del FRE se encarga de la consolidación de la información de los anexos. </t>
+  </si>
+  <si>
+    <t>1-7</t>
+  </si>
+  <si>
+    <t>Las copias de los recetarios oficiales allegados junto con los informes de las instituciones se almacenan en la bodega por un año. Los documentos digitales se almacenan en los equipos alrededor de 2 años antes de su eliminación.</t>
+  </si>
+  <si>
+    <t>Las instituciones inscritas envían sus informes de en los 10 primeros días del mes junto con las copias de los recetarios oficiales. Esto se envía en físico y por vía electrónica. Posterior a ello una regente de farmacia del FRE se encarga de la consolidación de la información de los anexos.</t>
+  </si>
+  <si>
+    <t>Una regente de farmacia se encarga de la consolidación de informes que llegan mensualmente. Esta labor le toma los diez primeros días del mes e incluso más en algunas ocasiones.</t>
+  </si>
+  <si>
+    <t>Llamada</t>
+  </si>
+  <si>
+    <t>Se lleva a cabo mediante los archivos de Microsoft Excel en donde se lleva el manejo de anexos de las resoluciones. Allí se contrasta los envíos del mes anterior con los actuales y así determinar que entidad está incumpliendo el envío de sus anexos.</t>
+  </si>
+  <si>
+    <t>No hay más establecimientos además del FRE que distribuyan MME</t>
+  </si>
+  <si>
+    <t>1-5</t>
+  </si>
+  <si>
+    <t>Rara vez</t>
+  </si>
+  <si>
+    <t>Andrés Alexander Benavides Salazar</t>
+  </si>
+  <si>
+    <t>Nariño</t>
+  </si>
+  <si>
+    <t>Pasto</t>
+  </si>
+  <si>
+    <t>Calle 15 No. 28 - 41 Plazuela de Bomboná</t>
+  </si>
+  <si>
+    <t>informesfrenarino@gmail.com, alexito5833@gmail.com</t>
+  </si>
+  <si>
+    <t>7223031 ext. 114.</t>
+  </si>
+  <si>
+    <t>No. 033 RESOLUCION DE CREACION
+CON MODIFICACION DESPUES POR LA RESOLUCION No. 0420 de 2011</t>
+  </si>
+  <si>
+    <t>Diana Paola Rosero Zambrano</t>
+  </si>
+  <si>
+    <t>Jhon Alexander Rojas Cabrera</t>
+  </si>
+  <si>
+    <t>Adriana Marcela Samudio Martinez</t>
+  </si>
+  <si>
+    <t>Luceny Del Rosario Gonzalez Mejia</t>
+  </si>
+  <si>
+    <t>Todo el proceso se centraliza en la oficina del Fondo Rotatorio. EL FRE empieza realizando las cotizaciones externas, para luego realizar el estudio de mercado. Esta información se pasa a la parte jurídica del FRE donde allí se encargan de realizar la elaboración del contrato. 
+El seguimiento de la revisión del contrato, las subastas y liquidación son hechas por el FRE.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De acuerdo al monto destinado que se tiene para la compra de los RO. Esta suma de dinero esta establecida bajo decreto. Por ejemplo, por decreto se definió el monto de $30’000.000 para la compra de RO, con ese dinero se puede comprar RO para dos o tres años, dependiendo del valor de compra de los talonarios. </t>
+  </si>
+  <si>
+    <t>Desde que se empieza a hacer la recolección de la información para las cotizaciones hasta la contratación del proveedor, pueden pasar de 2 a 3 meses. Desde que se acepta el contrato hasta que llegan los talonarios al FRE, pueden pasar de 15 a 30 días.</t>
+  </si>
+  <si>
+    <t>Resolución 2419 de 2006, modificada por la Resolución 67 de 2021.</t>
+  </si>
+  <si>
+    <t>Los interesados realizan la consignación a la cuenta del FRE. Luego, deben entregar el comprobante junto con dos copias en las oficinas del FRE, además deben traer el oficio de solicitud membretada de la institución. La persona encargada de solicitar los talonarios debe ser el representante legal, en caso contrario, debe traer carta de autorización. Después se realiza el registro de la compra y la respectiva entrega.</t>
+  </si>
+  <si>
+    <t>Hoja de cálculo, Libro contable</t>
+  </si>
+  <si>
+    <t>Tipo de persona (comprador), Unidades compradas, Venta total en moneda (COP), Fecha y hora, Otros</t>
+  </si>
+  <si>
+    <t>Número de factura</t>
+  </si>
+  <si>
+    <t>Se tiene un plan de contingencia verbal el cual consiste en realizar préstamos entre instituciones, es decir, la institución que tenga más RO, deberá prestar a las otras mientras se suple la necesidad. En caso de que haya nula disponibilidad, se enviara una carta de autorización al FNE para autorizar prescripciones normales.</t>
+  </si>
+  <si>
+    <t>Tiene puntos buenos y malos. Buenos porque la adquisición de RO es más fácil y oportuna. Malos porque no hay tanto control en cuanto al diligenciamiento del ROE.</t>
+  </si>
+  <si>
+    <t>Cuando ocurre una situación de estas, la información se pasa al área legal para realizar el respectivo proceso jurídico y/o sancionatorio.</t>
+  </si>
+  <si>
+    <t>Quincenal</t>
+  </si>
+  <si>
+    <t>Por medio de un formato en Excel y por medio del libro de registro de salidas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se revisa la letra, el color, el papel. </t>
+  </si>
+  <si>
+    <t>Marcas de agua, Fondos especiales (membretes), Microletras / microtexto, Sellos/Escudos, Codificación</t>
+  </si>
+  <si>
+    <t>Las instituciones allegan los informes con los RO, se debe radicar y lo allegan a la oficina principal del FRE. Allí se verifica que los RO sean las mismas en las salidas de la institución. Cuando la institución es nueva, se solicita la factura para el ingreso y las prescripciones, para las salidas.</t>
+  </si>
+  <si>
+    <t>Para hospitales hasta 4 horas.
+Servicios pequeños, 10 minutos.</t>
+  </si>
+  <si>
+    <t>Se destruyen para evitar el uso de espacios de la bodega.</t>
+  </si>
+  <si>
+    <t>Se realiza con el promedio de distribución de los últimos 6 meses, es decir, que porcentaje ha salido en esos meses.</t>
+  </si>
+  <si>
+    <t>Debido a la agilidad en los procesos de compra, puesto que antes se demoraban 4 meses realizando dicha acción, ahora, tarda por mucho un mes. Se sugiere seguir realizando las compras por esta plataforma de forma indefinida.</t>
+  </si>
+  <si>
+    <t>Se revisan todas las cajas.  Los MME son recibidos y se inspecciona cada una de las cajas, así mismo, se procede a revisar de donde provienen. También se revisa que las cantidades solicitadas sean las allegadas, junto con otras características. Después se revisa que los MME hayan llegado en óptimas condiciones. Sin embargo, no se tiene un proceso escrito para tal procedimiento, se está incursionando.</t>
+  </si>
+  <si>
+    <t>Cuando se encuentran productos no conformes durante la recepción técnica, el FRE envía un correo al FNE adjuntando fotos de la encontrado.</t>
+  </si>
+  <si>
+    <t>Almacenamiento en oficina privada, Inventario físico diario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dichas estrategias se encuentran en implementación </t>
+  </si>
+  <si>
+    <t>No se ha tenido inconvenientes con ningún operador, sea cual sea, siempre llegan rápido y sin inconvenientes.</t>
+  </si>
+  <si>
+    <t>El control de existencias se realiza diario y para llevar control de las fechas de vencimiento, colocan los MME con fechas lejanas de vencimiento en la parte de atrás del estante. En ocasiones, no se abren los empaques puesto que la fecha de vencimiento es lejana.</t>
+  </si>
+  <si>
+    <t>Para aproximadamente 6 meses.</t>
+  </si>
+  <si>
+    <t>No cuesta nada</t>
+  </si>
+  <si>
+    <t>El proceso de venta de MME a las instituciones se realiza igual al proceso de venta de RO, la única diferencia es que se piden las facturas y las prescripciones para comprar lo reportado en el RO.</t>
+  </si>
+  <si>
+    <t>Entre 3 a 6 meses.</t>
+  </si>
+  <si>
+    <t>Hasta el momento no se ha presentado una situación similar.</t>
+  </si>
+  <si>
+    <t>No se realiza dicha actividad.</t>
+  </si>
+  <si>
+    <t>Por medio de llamada telefónica con el responsable del FRE. Para los MCE se realiza transcripción.</t>
+  </si>
+  <si>
+    <t>Deben allegar copia de la historia clínica para realizar una trascripción a un RO.</t>
+  </si>
+  <si>
+    <t>El encargado del FRE, el señor Andres Benavides, se encarga de llenar dicho anexo teniendo en cuenta las facturas que salen.</t>
+  </si>
+  <si>
+    <t>De 6 a 24 horas</t>
+  </si>
+  <si>
+    <t>Dichos informes no se guardan en físico.</t>
+  </si>
+  <si>
+    <t>Este se realiza por medio de un software, el cual recopila la información y al momento de enviar la información al FNE, se descarga un archivo que se copia en una hoja de Excel.</t>
+  </si>
+  <si>
+    <t>Solo una persona.</t>
+  </si>
+  <si>
+    <t>Si, el libro contable y archivo de excel</t>
+  </si>
+  <si>
+    <t>Si se tiene, se solicitó durante el acompañamiento.</t>
+  </si>
+  <si>
+    <t>2 - 3</t>
+  </si>
+  <si>
+    <t>Omcomed y confamiliar.</t>
+  </si>
+  <si>
+    <t>NR</t>
+  </si>
+  <si>
+    <t>Silvia Espitia Vergara</t>
+  </si>
+  <si>
+    <t>Greici Castilla</t>
+  </si>
+  <si>
+    <t>Cauca</t>
+  </si>
+  <si>
+    <t>Popayán</t>
+  </si>
+  <si>
+    <t>Calle 5 # 15 – 57 Barrio Valencia Popayán  Sec Salud</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> silvia.espitia@saludcauca.gov.co</t>
+  </si>
+  <si>
+    <t>8209615/ 3145264278</t>
+  </si>
+  <si>
+    <t>Ordenanza No. 077 del 2008 /Resolución que asigna función 9712 del 29/12/2008</t>
+  </si>
+  <si>
+    <t>Lida Rosalba Mera</t>
+  </si>
+  <si>
+    <t>Elias Larraondo Carabalí</t>
+  </si>
+  <si>
+    <t>Greci Castilla</t>
+  </si>
+  <si>
+    <t>Silvia Sotelo</t>
+  </si>
+  <si>
+    <t>Donny Marín</t>
+  </si>
+  <si>
+    <t>Ingeniero de Sistemas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosalba Bravo </t>
+  </si>
+  <si>
+    <t>50-75</t>
+  </si>
+  <si>
+    <t>Ventas de medicamentos, Venta de recetarios, Recursos propios del FRE, Inscripciones-novedades establecimientos, Otras resoluciones (destrucciones, transformaciones)</t>
+  </si>
+  <si>
+    <t>Se alistan estudios previos y toda la solitud precontractual, se elabora registro presupuestal, la asignación se hace en la oficina del contratación, se hace asignación y se reciben en el almacén los recetarios, se tramita cuenta de cobro luego de la entrega,(elementos enteros), pago con una sola factura.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compras de 2000 unidades fijas, mandar a hacer 4000 en 2019, habitualmente 2000 en 2000, no hay una fórmula. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estudios previos 1 semana
+Etapa Contractual 3 meses
+</t>
+  </si>
+  <si>
+    <t>Resolución 06344 122020 del 31 de Dic del 2020</t>
+  </si>
+  <si>
+    <t>El FRE Cauca solo hace venta de 1 recetario por médico, por ejemplo si se vende 15 recetarios y se les debe hacer reposición se mira a que instituciones y a qué médicos. Se hace la cotización, luego la consignación. Se entregan inmediatamente. Oficio legal firmado por representante, relacionar los médicos con número de tarjeta profesional, consignación y se realiza entrega física. Las facturas manuales</t>
+  </si>
+  <si>
+    <t>Otros</t>
+  </si>
+  <si>
+    <t>REGISTRO REPS</t>
+  </si>
+  <si>
+    <t>Durante escasez y hasta nueva disponibilidad se podía autorizar prescripción en formulas médicas de las IPS. Se mandan a hacer con recursos propios, ya sucedió.</t>
+  </si>
+  <si>
+    <t>Simplifica procesos, pero también observan que puede ser un mecanismo que puede facilitar la fraudulencia, desconfianza en posibles desvíos.</t>
+  </si>
+  <si>
+    <t>Evaluación sobre el uso de recetarios, requisitos que ya mencionaron, contacto con habilitación, en ese caso ellos llaman al FRE y ellos visitan. Se revisa con que frecuencia anulan fórmulas. En cuantas formulas, cuan ven alguna novedad verifican, puede aumentar volúmenes de atenciones, pero se examina de manera rigurosa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Van mirando cajas, también con las visitas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se investiga la pérdida y se abre proceso sancionatorio, </t>
+  </si>
+  <si>
+    <t>Marcas de agua, Bande de seguridad, Filamentos de seguridad, Fluorescencia, Fondos especiales (membretes), Microletras / microtexto, Imagen latente, Relieve / laminado, Tinta invisibles o fluorescentes, Sellos/Escudos, Codificación</t>
+  </si>
+  <si>
+    <t>No se realiza proceso</t>
+  </si>
+  <si>
+    <t>LoS tiene cada IPS Y ELLOS SE ENCARGAN</t>
+  </si>
+  <si>
+    <t>3 de escritorio y ellos tienen sus propios computadores, falta uno para el ingenieros 6 computadores mínimo.</t>
+  </si>
+  <si>
+    <t>iNSUFICIENTES PARA EL FRE</t>
+  </si>
+  <si>
+    <t>Se calcula con base en consumo histórico y el comportamiento del año inmeditamente anterior de manera articulada con el FNE, sacan solicitud de disponibilidad Presupuestal y se hace la compra.</t>
+  </si>
+  <si>
+    <t>1-20</t>
+  </si>
+  <si>
+    <t>No hay queja alguna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procedimiento de recepción técnica está para aprobación, se llena formato de recepción técnica, tiene tres firmas para autorizar, regente de farmacia, recibe la factura, y la entrega del acta de entrada al almacén, se hace inspección física, empaques primarios y secundarios, que no hayan averías, si las hay notificar, </t>
+  </si>
+  <si>
+    <t>Si hay cualquier novedad de averías se notifica dentro de la misma acta y se informa al FNE para las reposiciones. Se pasan a proceso de cuarentena destrucción e incineración. Greci hace revisión de los documentos y los medicamentos, ya aprobada por Silvia</t>
+  </si>
+  <si>
+    <t>Gabinete con llave doble, Inventario físico diario</t>
+  </si>
+  <si>
+    <t>Termohigrómetro, Registro electrónico de condiciones</t>
+  </si>
+  <si>
+    <t>Aseguran que los medicamentos estén separados en concentraciones y cajas similares, se tienen rotulados los estantes.</t>
+  </si>
+  <si>
+    <t>Bastantes averías</t>
+  </si>
+  <si>
+    <t>Los productos que se vencen es porque hay mucha baja rotación</t>
+  </si>
+  <si>
+    <t>sI</t>
+  </si>
+  <si>
+    <t>Cajas fuera del almacén. Solicitud de ampliación no ha sido prioridad</t>
+  </si>
+  <si>
+    <t>Primidona 10mg</t>
+  </si>
+  <si>
+    <t>Hacen solicitud y se verifica con consumo e inventarios, se dispone del inventario, una vez se hace la respuesta a la cotización, se hace la consignación y se les da ese mismo día</t>
+  </si>
+  <si>
+    <t>130 inscritas, Todas compran</t>
+  </si>
+  <si>
+    <t>No hacen devoluciones, o hacen solicitud de rotación</t>
+  </si>
+  <si>
+    <t>Intervención a la institución, y se investiga si hay desabastecimiento.</t>
+  </si>
+  <si>
+    <t>Evalúan los casos, a través de particulares.</t>
+  </si>
+  <si>
+    <t>llamada al paciente visita domiciliaria</t>
+  </si>
+  <si>
+    <t>No ha sucedido.</t>
+  </si>
+  <si>
+    <t>Para medicamentos no MME se solicita transcripción.</t>
+  </si>
+  <si>
+    <t>No se ha recibido.</t>
+  </si>
+  <si>
+    <t>Ingeniero se encarga</t>
+  </si>
+  <si>
+    <t>Dos personas</t>
+  </si>
+  <si>
+    <t>Documentos físico</t>
+  </si>
+  <si>
+    <t>Se reciben los informes y se revisan, lo hace un regente  Los 5 primeros días de cada mes</t>
+  </si>
+  <si>
+    <t>Se hace a mano</t>
+  </si>
+  <si>
+    <t>Todo el FRE</t>
+  </si>
+  <si>
+    <t>Archivos AZ/Bases de Excel</t>
+  </si>
+  <si>
+    <t>Se están estandarizando procesos, próximos a aprobación.</t>
+  </si>
+  <si>
+    <t>Compras semestrales</t>
+  </si>
+  <si>
+    <t>No se hace.</t>
+  </si>
+  <si>
+    <t>0-20</t>
+  </si>
+  <si>
+    <t>Guaviare</t>
+  </si>
+  <si>
+    <t>Putumayo</t>
+  </si>
+  <si>
+    <t>Mocoa</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
@@ -3234,7 +4025,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -3253,6 +4044,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3472,17 +4270,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:FY13"/>
+  <dimension ref="A1:FY17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="BK2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BM1" sqref="BM1"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4338,7 +5136,7 @@
       <c r="DQ2" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="DR2" s="2" t="s">
+      <c r="DR2" s="12" t="s">
         <v>225</v>
       </c>
       <c r="DS2" s="2" t="s">
@@ -4359,7 +5157,7 @@
       <c r="DX2" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="DY2" s="2" t="s">
+      <c r="DY2" s="12" t="s">
         <v>231</v>
       </c>
       <c r="DZ2" s="2" t="s">
@@ -4386,13 +5184,13 @@
       <c r="EG2" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="EH2" s="2" t="s">
+      <c r="EH2" s="8" t="s">
         <v>237</v>
       </c>
       <c r="EI2" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="EJ2" s="2" t="s">
+      <c r="EJ2" s="12" t="s">
         <v>239</v>
       </c>
       <c r="EK2" s="2" t="s">
@@ -4754,7 +5552,7 @@
       <c r="DQ3" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="DR3" s="2" t="s">
+      <c r="DR3" s="12" t="s">
         <v>197</v>
       </c>
       <c r="DT3" s="2" t="s">
@@ -4772,7 +5570,7 @@
       <c r="DX3" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="DY3" s="2" t="s">
+      <c r="DY3" s="12" t="s">
         <v>231</v>
       </c>
       <c r="DZ3" s="2" t="s">
@@ -4802,7 +5600,7 @@
       <c r="EI3" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="EJ3" s="2" t="s">
+      <c r="EJ3" s="12" t="s">
         <v>314</v>
       </c>
       <c r="EK3" s="2" t="s">
@@ -5150,7 +5948,7 @@
       <c r="DQ4" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="DR4" s="2" t="s">
+      <c r="DR4" s="12" t="s">
         <v>225</v>
       </c>
       <c r="DS4" s="2" t="s">
@@ -5171,7 +5969,7 @@
       <c r="DX4" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="DY4" s="2" t="s">
+      <c r="DY4" s="12" t="s">
         <v>231</v>
       </c>
       <c r="DZ4" s="2" t="s">
@@ -5192,13 +5990,13 @@
       <c r="EG4" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="EH4" s="2" t="s">
+      <c r="EH4" s="8" t="s">
         <v>383</v>
       </c>
       <c r="EI4" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="EJ4" s="2" t="s">
+      <c r="EJ4" s="12" t="s">
         <v>385</v>
       </c>
       <c r="EK4" s="2" t="s">
@@ -5549,7 +6347,7 @@
       <c r="DQ5" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="DR5" s="2" t="s">
+      <c r="DR5" s="12" t="s">
         <v>442</v>
       </c>
       <c r="DT5" s="2" t="s">
@@ -5567,7 +6365,7 @@
       <c r="DX5" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="DY5" s="2" t="s">
+      <c r="DY5" s="12" t="s">
         <v>231</v>
       </c>
       <c r="DZ5" s="2" t="s">
@@ -5597,7 +6395,7 @@
       <c r="EI5" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="EJ5" s="2" t="s">
+      <c r="EJ5" s="12" t="s">
         <v>346</v>
       </c>
       <c r="EK5" s="2" t="s">
@@ -5996,7 +6794,7 @@
       <c r="DQ6" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="DR6" s="2" t="s">
+      <c r="DR6" s="12" t="s">
         <v>442</v>
       </c>
       <c r="DT6" s="2" t="s">
@@ -6014,7 +6812,7 @@
       <c r="DX6" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="DY6" s="2" t="s">
+      <c r="DY6" s="12" t="s">
         <v>231</v>
       </c>
       <c r="DZ6" s="2" t="s">
@@ -6044,7 +6842,7 @@
       <c r="EI6" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="EJ6" s="2" t="s">
+      <c r="EJ6" s="12" t="s">
         <v>517</v>
       </c>
       <c r="EK6" s="2" t="s">
@@ -6446,7 +7244,7 @@
       <c r="DQ7" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="DR7" s="2" t="s">
+      <c r="DR7" s="12" t="s">
         <v>574</v>
       </c>
       <c r="DT7" s="2" t="s">
@@ -6464,7 +7262,7 @@
       <c r="DX7" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="DY7" s="2" t="s">
+      <c r="DY7" s="12" t="s">
         <v>231</v>
       </c>
       <c r="DZ7" s="2" t="s">
@@ -6485,13 +7283,13 @@
       <c r="EG7" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="EH7" s="2" t="s">
+      <c r="EH7" s="8" t="s">
         <v>582</v>
       </c>
       <c r="EI7" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="EJ7" s="2" t="s">
+      <c r="EJ7" s="12" t="s">
         <v>583</v>
       </c>
       <c r="EK7" s="2" t="s">
@@ -6869,7 +7667,7 @@
       <c r="DX8" s="2" t="s">
         <v>642</v>
       </c>
-      <c r="DY8" s="2" t="s">
+      <c r="DY8" s="12" t="s">
         <v>231</v>
       </c>
       <c r="DZ8" s="2" t="s">
@@ -6893,13 +7691,13 @@
       <c r="EG8" s="2" t="s">
         <v>647</v>
       </c>
-      <c r="EH8" s="2" t="s">
+      <c r="EH8" s="8" t="s">
         <v>648</v>
       </c>
       <c r="EI8" s="2" t="s">
         <v>649</v>
       </c>
-      <c r="EJ8" s="2" t="s">
+      <c r="EJ8" s="12" t="s">
         <v>608</v>
       </c>
       <c r="EK8" s="2" t="s">
@@ -7328,7 +8126,7 @@
       <c r="DX9" s="2" t="s">
         <v>720</v>
       </c>
-      <c r="DY9" s="2" t="s">
+      <c r="DY9" s="12" t="s">
         <v>231</v>
       </c>
       <c r="DZ9" s="2" t="s">
@@ -7355,7 +8153,7 @@
       <c r="EI9" s="2" t="s">
         <v>726</v>
       </c>
-      <c r="EJ9" s="2" t="s">
+      <c r="EJ9" s="12" t="s">
         <v>727</v>
       </c>
       <c r="EK9" s="2" t="s">
@@ -7749,7 +8547,7 @@
       <c r="DX10" s="2" t="s">
         <v>779</v>
       </c>
-      <c r="DY10" s="2" t="s">
+      <c r="DY10" s="12" t="s">
         <v>231</v>
       </c>
       <c r="DZ10" s="2" t="s">
@@ -7770,13 +8568,13 @@
       <c r="EG10" s="2" t="s">
         <v>783</v>
       </c>
-      <c r="EH10" s="2" t="s">
+      <c r="EH10" s="8" t="s">
         <v>784</v>
       </c>
       <c r="EI10" s="2" t="s">
         <v>785</v>
       </c>
-      <c r="EJ10" s="2" t="s">
+      <c r="EJ10" s="12" t="s">
         <v>786</v>
       </c>
       <c r="EK10" s="2" t="s">
@@ -8176,7 +8974,7 @@
       <c r="DX11" s="2" t="s">
         <v>836</v>
       </c>
-      <c r="DY11" s="2" t="s">
+      <c r="DY11" s="12" t="s">
         <v>231</v>
       </c>
       <c r="DZ11" s="2" t="s">
@@ -8206,7 +9004,7 @@
       <c r="EI11" s="2" t="s">
         <v>842</v>
       </c>
-      <c r="EJ11" s="2" t="s">
+      <c r="EJ11" s="12" t="s">
         <v>812</v>
       </c>
       <c r="EK11" s="2" t="s">
@@ -8629,7 +9427,7 @@
       <c r="DX12" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="DY12" s="2" t="s">
+      <c r="DY12" s="12" t="s">
         <v>197</v>
       </c>
       <c r="DZ12" s="2" t="s">
@@ -8656,7 +9454,7 @@
       <c r="EI12" s="2" t="s">
         <v>902</v>
       </c>
-      <c r="EJ12" s="2" t="s">
+      <c r="EJ12" s="12" t="s">
         <v>903</v>
       </c>
       <c r="EK12" s="2" t="s">
@@ -9079,7 +9877,7 @@
       <c r="DX13" s="2" t="s">
         <v>596</v>
       </c>
-      <c r="DY13" s="2" t="s">
+      <c r="DY13" s="12" t="s">
         <v>231</v>
       </c>
       <c r="DZ13" s="2" t="s">
@@ -9109,7 +9907,7 @@
       <c r="EI13" s="2" t="s">
         <v>968</v>
       </c>
-      <c r="EJ13" s="2" t="s">
+      <c r="EJ13" s="12" t="s">
         <v>198</v>
       </c>
       <c r="EK13" s="2" t="s">
@@ -9225,6 +10023,1742 @@
       </c>
       <c r="FY13" s="2" t="s">
         <v>471</v>
+      </c>
+    </row>
+    <row r="14" spans="1:181" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="18">
+        <v>44370.575993657403</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="E14" s="19">
+        <v>44363</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>1225</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>984</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="J14" s="1">
+        <v>3213946562</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="L14" s="19">
+        <v>41869</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>988</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="Z14" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AA14" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="AB14" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AD14" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="AE14" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AG14" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AI14" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="AJ14" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AL14" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AN14" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="AO14" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AP14" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="AR14" s="1">
+        <v>5250</v>
+      </c>
+      <c r="AS14" s="1">
+        <v>800</v>
+      </c>
+      <c r="AT14" s="1">
+        <v>27</v>
+      </c>
+      <c r="AU14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AV14" s="1">
+        <v>50</v>
+      </c>
+      <c r="AW14" s="1">
+        <v>18000</v>
+      </c>
+      <c r="AX14" s="1">
+        <v>25000</v>
+      </c>
+      <c r="AY14" s="1">
+        <v>500</v>
+      </c>
+      <c r="BA14" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="BD14" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="BE14" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="BF14" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="BG14" s="1">
+        <v>14</v>
+      </c>
+      <c r="BH14" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="BI14" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="BJ14" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="BK14" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="BM14" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="BN14" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="BO14" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="BP14" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="BQ14" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="BR14" s="1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="BS14" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="BT14" s="1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="BU14" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="BW14" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="BX14" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="BY14" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="BZ14" s="1" t="s">
+        <v>1011</v>
+      </c>
+      <c r="CA14" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="CB14" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="CD14" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="CE14" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="CF14" s="1" t="s">
+        <v>1013</v>
+      </c>
+      <c r="CG14" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="CH14" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="CJ14" s="1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="CK14" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="CL14" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="CM14" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="CO14" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="CQ14" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="CS14" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="CT14" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="CU14" s="1">
+        <v>1</v>
+      </c>
+      <c r="CV14" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="CX14" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="CY14" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="CZ14" s="1">
+        <v>3</v>
+      </c>
+      <c r="DA14" s="1">
+        <v>2</v>
+      </c>
+      <c r="DB14" s="1">
+        <v>6</v>
+      </c>
+      <c r="DC14" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="DD14" s="1">
+        <v>4</v>
+      </c>
+      <c r="DE14" s="1">
+        <v>3</v>
+      </c>
+      <c r="DF14" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="DG14" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="DH14" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="DI14" s="1">
+        <v>1</v>
+      </c>
+      <c r="DJ14" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="DK14" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="DM14" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="DN14" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="DP14" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="DQ14" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="DR14" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="DT14" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="DU14" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="DV14" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="DW14" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="DX14" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="DY14" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="DZ14" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="EA14" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="EC14" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="ED14" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="EE14" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="EF14" s="1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="EG14" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="EH14" s="1">
+        <v>6</v>
+      </c>
+      <c r="EI14" s="1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="EJ14" s="24" t="s">
+        <v>608</v>
+      </c>
+      <c r="EK14" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="EL14" s="1" t="s">
+        <v>1034</v>
+      </c>
+      <c r="EM14" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="EO14" s="1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="EP14" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="EQ14" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="ER14" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="ES14" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="ET14" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="EU14" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="EW14" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="EX14" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="EY14" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="EZ14" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="FA14" s="1" t="s">
+        <v>1041</v>
+      </c>
+      <c r="FB14" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="FC14" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="FD14" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="FE14" s="1" t="s">
+        <v>1043</v>
+      </c>
+      <c r="FF14" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="FH14" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="FI14" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="FJ14" s="1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="FK14" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="FL14" s="1">
+        <v>2</v>
+      </c>
+      <c r="FM14" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="FN14" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="FO14" s="1">
+        <v>1</v>
+      </c>
+      <c r="FP14" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="FQ14" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="FR14" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="FS14" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="FT14" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="FU14" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="FV14" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="FY14" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="15" spans="1:181" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="18">
+        <v>44384.71444163195</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E15" s="19">
+        <v>44363</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>1226</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>1227</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="J15" s="1">
+        <v>3143405646</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>1049</v>
+      </c>
+      <c r="L15" s="19">
+        <v>40816</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>1053</v>
+      </c>
+      <c r="Z15" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AB15" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AR15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS15" s="1">
+        <v>90</v>
+      </c>
+      <c r="AT15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU15" s="1">
+        <v>3</v>
+      </c>
+      <c r="AV15" s="1">
+        <v>25</v>
+      </c>
+      <c r="AW15" s="1">
+        <v>15000</v>
+      </c>
+      <c r="AX15" s="1">
+        <v>29000</v>
+      </c>
+      <c r="AY15" s="1">
+        <v>1160</v>
+      </c>
+      <c r="BA15" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="BD15" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="BE15" s="1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="BF15" s="1" t="s">
+        <v>1055</v>
+      </c>
+      <c r="BG15" s="1">
+        <v>240</v>
+      </c>
+      <c r="BH15" s="1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="BI15" s="1" t="s">
+        <v>1057</v>
+      </c>
+      <c r="BJ15" s="1" t="s">
+        <v>1058</v>
+      </c>
+      <c r="BK15" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="BL15" s="1" t="s">
+        <v>1059</v>
+      </c>
+      <c r="BM15" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="BO15" s="1" t="s">
+        <v>1061</v>
+      </c>
+      <c r="BP15" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="BQ15" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="BR15" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="BT15" s="1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="BU15" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="BW15" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="BX15" s="1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="BY15" s="1" t="s">
+        <v>1065</v>
+      </c>
+      <c r="CA15" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="CB15" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="CD15" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="CE15" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="CF15" s="1" t="s">
+        <v>1067</v>
+      </c>
+      <c r="CG15" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="CH15" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="CJ15" s="1" t="s">
+        <v>1068</v>
+      </c>
+      <c r="CK15" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="CL15" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="CM15" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="CO15" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="CP15" s="1" t="s">
+        <v>1069</v>
+      </c>
+      <c r="CQ15" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="CS15" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="CT15" s="1" t="s">
+        <v>1070</v>
+      </c>
+      <c r="CU15" s="1">
+        <v>2</v>
+      </c>
+      <c r="CV15" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="CW15" s="1" t="s">
+        <v>1071</v>
+      </c>
+      <c r="CX15" s="1" t="s">
+        <v>1072</v>
+      </c>
+      <c r="CY15" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="CZ15" s="1">
+        <v>5</v>
+      </c>
+      <c r="DA15" s="1">
+        <v>10</v>
+      </c>
+      <c r="DB15" s="1">
+        <v>30</v>
+      </c>
+      <c r="DC15" s="1">
+        <v>4</v>
+      </c>
+      <c r="DD15" s="1">
+        <v>7</v>
+      </c>
+      <c r="DE15" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="DF15" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="DG15" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="DH15" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="DI15" s="21" t="s">
+        <v>1076</v>
+      </c>
+      <c r="DJ15" s="1" t="s">
+        <v>1077</v>
+      </c>
+      <c r="DK15" s="1" t="s">
+        <v>1078</v>
+      </c>
+      <c r="DM15" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="DN15" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="DP15" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="DQ15" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="DR15" s="1" t="s">
+        <v>1080</v>
+      </c>
+      <c r="DT15" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="DU15" s="1" t="s">
+        <v>1081</v>
+      </c>
+      <c r="DV15" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="DW15" s="1" t="s">
+        <v>1082</v>
+      </c>
+      <c r="DX15" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="DY15" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="DZ15" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="EA15" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="EC15" s="1" t="s">
+        <v>1083</v>
+      </c>
+      <c r="ED15" s="1" t="s">
+        <v>1084</v>
+      </c>
+      <c r="EE15" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="EF15" s="1" t="s">
+        <v>1085</v>
+      </c>
+      <c r="EG15" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="EH15" s="1">
+        <v>43</v>
+      </c>
+      <c r="EI15" s="1" t="s">
+        <v>1087</v>
+      </c>
+      <c r="EJ15" s="24">
+        <v>0</v>
+      </c>
+      <c r="EK15" s="1" t="s">
+        <v>1088</v>
+      </c>
+      <c r="EL15" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="EM15" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="EO15" s="1" t="s">
+        <v>1090</v>
+      </c>
+      <c r="EP15" s="1" t="s">
+        <v>1091</v>
+      </c>
+      <c r="EQ15" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="ER15" s="1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="ES15" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="ET15" s="21" t="s">
+        <v>1094</v>
+      </c>
+      <c r="EU15" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="EW15" s="1" t="s">
+        <v>1095</v>
+      </c>
+      <c r="EX15" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="EY15" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="EZ15" s="1" t="s">
+        <v>1096</v>
+      </c>
+      <c r="FA15" s="1" t="s">
+        <v>1097</v>
+      </c>
+      <c r="FB15" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="FC15" s="1" t="s">
+        <v>1098</v>
+      </c>
+      <c r="FD15" s="1" t="s">
+        <v>1099</v>
+      </c>
+      <c r="FE15" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="FF15" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="FH15" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="FI15" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="FJ15" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="FL15" s="21" t="s">
+        <v>1076</v>
+      </c>
+      <c r="FM15" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="FN15" s="1" t="s">
+        <v>1100</v>
+      </c>
+      <c r="FO15" s="21" t="s">
+        <v>1101</v>
+      </c>
+      <c r="FP15" s="1" t="s">
+        <v>1102</v>
+      </c>
+      <c r="FQ15" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="FR15" s="22">
+        <v>0.15</v>
+      </c>
+      <c r="FS15" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="FT15" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="FU15" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="FV15" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="FX15" s="1" t="s">
+        <v>1069</v>
+      </c>
+      <c r="FY15" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="16" spans="1:181" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="18">
+        <v>44385.476659016203</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>1103</v>
+      </c>
+      <c r="E16" s="19">
+        <v>44363</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>1105</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>1106</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>1107</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>1108</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>1109</v>
+      </c>
+      <c r="L16" s="19">
+        <v>40602</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>1110</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>1111</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>1103</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>1112</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>1113</v>
+      </c>
+      <c r="Z16" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AB16" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AR16" s="1">
+        <v>6321</v>
+      </c>
+      <c r="AS16" s="1">
+        <v>175</v>
+      </c>
+      <c r="AT16" s="1">
+        <v>130</v>
+      </c>
+      <c r="AU16" s="1">
+        <v>3</v>
+      </c>
+      <c r="AV16" s="1">
+        <v>50</v>
+      </c>
+      <c r="AW16" s="1">
+        <v>3508</v>
+      </c>
+      <c r="AX16" s="1">
+        <v>28400</v>
+      </c>
+      <c r="AY16" s="1">
+        <v>70</v>
+      </c>
+      <c r="BA16" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="BD16" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="BE16" s="1" t="s">
+        <v>1114</v>
+      </c>
+      <c r="BF16" s="1" t="s">
+        <v>1115</v>
+      </c>
+      <c r="BG16" s="1">
+        <v>15</v>
+      </c>
+      <c r="BH16" s="1" t="s">
+        <v>1116</v>
+      </c>
+      <c r="BI16" s="1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="BJ16" s="1" t="s">
+        <v>1118</v>
+      </c>
+      <c r="BK16" s="1" t="s">
+        <v>1119</v>
+      </c>
+      <c r="BM16" s="1" t="s">
+        <v>1120</v>
+      </c>
+      <c r="BN16" s="1" t="s">
+        <v>1121</v>
+      </c>
+      <c r="BO16" s="1" t="s">
+        <v>1122</v>
+      </c>
+      <c r="BP16" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="BQ16" s="1" t="s">
+        <v>1123</v>
+      </c>
+      <c r="BR16" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="BT16" s="1" t="s">
+        <v>1124</v>
+      </c>
+      <c r="BU16" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="BV16" s="1" t="s">
+        <v>1125</v>
+      </c>
+      <c r="BW16" s="1" t="s">
+        <v>1126</v>
+      </c>
+      <c r="BX16" s="1" t="s">
+        <v>1127</v>
+      </c>
+      <c r="BY16" s="1" t="s">
+        <v>1128</v>
+      </c>
+      <c r="CA16" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="CB16" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="CD16" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="CE16" s="1" t="s">
+        <v>1129</v>
+      </c>
+      <c r="CF16" s="1" t="s">
+        <v>1130</v>
+      </c>
+      <c r="CG16" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="CH16" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="CJ16" s="1" t="s">
+        <v>1131</v>
+      </c>
+      <c r="CK16" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="CL16" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="CM16" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="CO16" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="CQ16" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="CS16" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="CT16" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="CU16" s="1">
+        <v>8</v>
+      </c>
+      <c r="CV16" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="CX16" s="1" t="s">
+        <v>1132</v>
+      </c>
+      <c r="CY16" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="CZ16" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="DA16" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="DB16" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="DC16" s="1">
+        <v>2</v>
+      </c>
+      <c r="DD16" s="1">
+        <v>3</v>
+      </c>
+      <c r="DE16" s="1">
+        <v>3</v>
+      </c>
+      <c r="DF16" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="DG16" s="1" t="s">
+        <v>1133</v>
+      </c>
+      <c r="DH16" s="1" t="s">
+        <v>1134</v>
+      </c>
+      <c r="DI16" s="1">
+        <v>1</v>
+      </c>
+      <c r="DJ16" s="1" t="s">
+        <v>1135</v>
+      </c>
+      <c r="DK16" s="1" t="s">
+        <v>1136</v>
+      </c>
+      <c r="DM16" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="DN16" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="DP16" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="DQ16" s="1" t="s">
+        <v>1137</v>
+      </c>
+      <c r="DR16" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="DT16" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="DU16" s="1" t="s">
+        <v>1138</v>
+      </c>
+      <c r="DV16" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="DW16" s="1" t="s">
+        <v>1139</v>
+      </c>
+      <c r="DX16" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="DY16" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="DZ16" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="EA16" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="EC16" s="1" t="s">
+        <v>1140</v>
+      </c>
+      <c r="ED16" s="1" t="s">
+        <v>1141</v>
+      </c>
+      <c r="EE16" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="EG16" s="1" t="s">
+        <v>1142</v>
+      </c>
+      <c r="EH16" s="1">
+        <v>220</v>
+      </c>
+      <c r="EI16" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="EJ16" s="24" t="s">
+        <v>1143</v>
+      </c>
+      <c r="EK16" s="1" t="s">
+        <v>1144</v>
+      </c>
+      <c r="EL16" s="1" t="s">
+        <v>1145</v>
+      </c>
+      <c r="EM16" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="EO16" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="EP16" s="1" t="s">
+        <v>1146</v>
+      </c>
+      <c r="EQ16" s="1" t="s">
+        <v>1147</v>
+      </c>
+      <c r="ER16" s="1" t="s">
+        <v>1148</v>
+      </c>
+      <c r="ES16" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="ET16" s="1" t="s">
+        <v>1149</v>
+      </c>
+      <c r="EU16" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="EW16" s="1" t="s">
+        <v>1150</v>
+      </c>
+      <c r="EX16" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="EY16" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="EZ16" s="1" t="s">
+        <v>1151</v>
+      </c>
+      <c r="FA16" s="1" t="s">
+        <v>1152</v>
+      </c>
+      <c r="FB16" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="FC16" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="FD16" s="1" t="s">
+        <v>1153</v>
+      </c>
+      <c r="FE16" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="FF16" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="FH16" s="1" t="s">
+        <v>1154</v>
+      </c>
+      <c r="FI16" s="1" t="s">
+        <v>1154</v>
+      </c>
+      <c r="FJ16" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="FL16" s="1" t="s">
+        <v>1155</v>
+      </c>
+      <c r="FM16" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="FN16" s="1" t="s">
+        <v>1156</v>
+      </c>
+      <c r="FO16" s="1">
+        <v>1</v>
+      </c>
+      <c r="FP16" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="FQ16" s="1" t="s">
+        <v>1157</v>
+      </c>
+      <c r="FR16" s="1" t="s">
+        <v>1157</v>
+      </c>
+      <c r="FS16" s="1" t="s">
+        <v>1157</v>
+      </c>
+      <c r="FT16" s="1" t="s">
+        <v>1157</v>
+      </c>
+      <c r="FU16" s="1" t="s">
+        <v>1157</v>
+      </c>
+      <c r="FV16" s="1" t="s">
+        <v>1157</v>
+      </c>
+      <c r="FY16" s="1" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="17" spans="1:181" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="18">
+        <v>44385.485729236112</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E17" s="19">
+        <v>44363</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>1160</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>1161</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>1162</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>1163</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>1164</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>1165</v>
+      </c>
+      <c r="L17" s="19">
+        <v>39783</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>1166</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>1167</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>1158</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>1168</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>1169</v>
+      </c>
+      <c r="Z17" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AA17" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="AB17" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AD17" s="1" t="s">
+        <v>1170</v>
+      </c>
+      <c r="AE17" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AF17" s="1" t="s">
+        <v>1171</v>
+      </c>
+      <c r="AG17" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AI17" s="1" t="s">
+        <v>1172</v>
+      </c>
+      <c r="AJ17" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AL17" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AR17" s="1">
+        <v>1950</v>
+      </c>
+      <c r="AS17" s="1" t="s">
+        <v>1173</v>
+      </c>
+      <c r="AT17" s="1">
+        <v>81</v>
+      </c>
+      <c r="AU17" s="1">
+        <v>3</v>
+      </c>
+      <c r="AV17" s="1">
+        <v>100</v>
+      </c>
+      <c r="AW17" s="1">
+        <v>17000</v>
+      </c>
+      <c r="AX17" s="1">
+        <v>3000</v>
+      </c>
+      <c r="AY17" s="1">
+        <v>300</v>
+      </c>
+      <c r="BA17" s="1" t="s">
+        <v>1174</v>
+      </c>
+      <c r="BD17" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="BE17" s="1" t="s">
+        <v>1175</v>
+      </c>
+      <c r="BF17" s="1" t="s">
+        <v>1176</v>
+      </c>
+      <c r="BG17" s="1">
+        <v>90</v>
+      </c>
+      <c r="BH17" s="1" t="s">
+        <v>1177</v>
+      </c>
+      <c r="BI17" s="1" t="s">
+        <v>1178</v>
+      </c>
+      <c r="BJ17" s="1" t="s">
+        <v>1179</v>
+      </c>
+      <c r="BK17" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="BM17" s="1" t="s">
+        <v>1180</v>
+      </c>
+      <c r="BN17" s="1" t="s">
+        <v>1181</v>
+      </c>
+      <c r="BO17" s="1" t="s">
+        <v>1182</v>
+      </c>
+      <c r="BP17" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="BQ17" s="1" t="s">
+        <v>1183</v>
+      </c>
+      <c r="BR17" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="BT17" s="1" t="s">
+        <v>1184</v>
+      </c>
+      <c r="BU17" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="BW17" s="1" t="s">
+        <v>1185</v>
+      </c>
+      <c r="BX17" s="1" t="s">
+        <v>1186</v>
+      </c>
+      <c r="BY17" s="1" t="s">
+        <v>1187</v>
+      </c>
+      <c r="CA17" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="CB17" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="CD17" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="CE17" s="1" t="s">
+        <v>1188</v>
+      </c>
+      <c r="CF17" s="1" t="s">
+        <v>1188</v>
+      </c>
+      <c r="CG17" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="CH17" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="CJ17" s="1" t="s">
+        <v>1189</v>
+      </c>
+      <c r="CK17" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="CL17" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="CM17" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="CO17" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="CQ17" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="CS17" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="CT17" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="CU17" s="1" t="s">
+        <v>1190</v>
+      </c>
+      <c r="CV17" s="1" t="s">
+        <v>1191</v>
+      </c>
+      <c r="CX17" s="1" t="s">
+        <v>1192</v>
+      </c>
+      <c r="CY17" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="CZ17" s="1">
+        <v>7</v>
+      </c>
+      <c r="DA17" s="1">
+        <v>12</v>
+      </c>
+      <c r="DB17" s="1" t="s">
+        <v>1193</v>
+      </c>
+      <c r="DC17" s="1">
+        <v>1</v>
+      </c>
+      <c r="DD17" s="1">
+        <v>13</v>
+      </c>
+      <c r="DE17" s="21" t="s">
+        <v>506</v>
+      </c>
+      <c r="DF17" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="DG17" s="1" t="s">
+        <v>1194</v>
+      </c>
+      <c r="DH17" s="1" t="s">
+        <v>1195</v>
+      </c>
+      <c r="DI17" s="21" t="s">
+        <v>1076</v>
+      </c>
+      <c r="DJ17" s="1" t="s">
+        <v>1196</v>
+      </c>
+      <c r="DK17" s="1" t="s">
+        <v>1197</v>
+      </c>
+      <c r="DM17" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="DN17" s="1" t="s">
+        <v>1198</v>
+      </c>
+      <c r="DP17" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="DQ17" s="1" t="s">
+        <v>1199</v>
+      </c>
+      <c r="DR17" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="DT17" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="DU17" s="1" t="s">
+        <v>1200</v>
+      </c>
+      <c r="DV17" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="DW17" s="1" t="s">
+        <v>1201</v>
+      </c>
+      <c r="DX17" s="1" t="s">
+        <v>1202</v>
+      </c>
+      <c r="DY17" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="DZ17" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="EA17" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="EC17" s="1" t="s">
+        <v>1203</v>
+      </c>
+      <c r="ED17" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="EE17" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="EF17" s="1" t="s">
+        <v>1204</v>
+      </c>
+      <c r="EG17" s="1" t="s">
+        <v>1205</v>
+      </c>
+      <c r="EH17" s="1" t="s">
+        <v>1206</v>
+      </c>
+      <c r="EI17" s="1" t="s">
+        <v>1207</v>
+      </c>
+      <c r="EJ17" s="24">
+        <v>1</v>
+      </c>
+      <c r="EK17" s="1" t="s">
+        <v>1208</v>
+      </c>
+      <c r="EL17" s="1" t="s">
+        <v>1209</v>
+      </c>
+      <c r="EM17" s="1" t="s">
+        <v>1210</v>
+      </c>
+      <c r="EO17" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="EP17" s="1" t="s">
+        <v>1212</v>
+      </c>
+      <c r="EQ17" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="ER17" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="ES17" s="1" t="s">
+        <v>1215</v>
+      </c>
+      <c r="ET17" s="1">
+        <v>3</v>
+      </c>
+      <c r="EU17" s="1" t="s">
+        <v>1216</v>
+      </c>
+      <c r="EW17" s="1" t="s">
+        <v>1217</v>
+      </c>
+      <c r="EX17" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="EY17" s="1" t="s">
+        <v>1215</v>
+      </c>
+      <c r="EZ17" s="1" t="s">
+        <v>1218</v>
+      </c>
+      <c r="FA17" s="1" t="s">
+        <v>1219</v>
+      </c>
+      <c r="FB17" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="FC17" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="FD17" s="1" t="s">
+        <v>1220</v>
+      </c>
+      <c r="FE17" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="FF17" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="FH17" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="FI17" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="FJ17" s="1" t="s">
+        <v>1221</v>
+      </c>
+      <c r="FL17" s="1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="FM17" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="FN17" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="FO17" s="1">
+        <v>1</v>
+      </c>
+      <c r="FP17" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="FQ17" s="22">
+        <v>0.4</v>
+      </c>
+      <c r="FR17" s="22">
+        <v>0.1</v>
+      </c>
+      <c r="FS17" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="FT17" s="1">
+        <v>0</v>
+      </c>
+      <c r="FU17" s="1">
+        <v>0</v>
+      </c>
+      <c r="FV17" s="1">
+        <v>0</v>
+      </c>
+      <c r="FY17" s="1" t="s">
+        <v>1224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se arreglan análisis de no de personas e instituciones inscritas
</commit_message>
<xml_diff>
--- a/data/intermediate/001_Herramienta_Limpieza_Manual.xlsx
+++ b/data/intermediate/001_Herramienta_Limpieza_Manual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\OneDrive\Documents\Trabajos\UAS-FNE-2\61_Regionalizacion\FRE_AnalisisEstadistico\data\intermediate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFFAB21-954A-4963-98FA-313A2C8B0AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA746EA-E9BE-4C80-A0F5-CD4404011D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -304,7 +304,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EI2" authorId="0" shapeId="0" xr:uid="{63FCDCEA-425C-4EC7-AAED-D528A07B9487}">
+    <comment ref="EI2" authorId="0" shapeId="0" xr:uid="{6FE0336A-0AD1-4736-A6F2-4FA3360E662E}">
       <text>
         <r>
           <rPr>
@@ -324,7 +324,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Decía: "Dato en bases de datos"</t>
+Decía dato en base datos</t>
         </r>
       </text>
     </comment>
@@ -856,7 +856,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EI4" authorId="0" shapeId="0" xr:uid="{BABA5DDC-4305-4DFD-8004-56BD70F8D114}">
+    <comment ref="EI4" authorId="0" shapeId="0" xr:uid="{A0193806-C2CF-4DF8-BCE7-1A558A3E4376}">
       <text>
         <r>
           <rPr>
@@ -2053,30 +2053,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="EI9" authorId="0" shapeId="0" xr:uid="{2877A2DE-5840-40E0-8497-56BE1CFCFC37}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Daniel S. Parra G.:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-34 establecimientos.</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="EU9" authorId="0" shapeId="0" xr:uid="{BE529271-7829-4F16-8648-565ECD8A1E8A}">
       <text>
         <r>
@@ -3472,30 +3448,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="EI16" authorId="0" shapeId="0" xr:uid="{A70B17BB-F63C-47DF-ADBE-90FF36A7D839}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Daniel S. Parra G.:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-130 inscritas, Todas compran</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="EU16" authorId="0" shapeId="0" xr:uid="{F759B86F-1951-45C8-8D35-4D27D55FD7CB}">
       <text>
         <r>
@@ -4219,6 +4171,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="EI20" authorId="0" shapeId="0" xr:uid="{5AC2EAE5-DC20-4839-991D-EF6E6A4506FE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Daniel S. Parra G.:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+No respondieron durante la encuesta.
+En anexos 2 se tenía 163-433</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="GG20" authorId="0" shapeId="0" xr:uid="{1B5BEB03-1DD9-49D5-82F1-6973500C4257}">
       <text>
         <r>
@@ -4339,30 +4316,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="EI21" authorId="0" shapeId="0" xr:uid="{DA2D6097-9192-426D-A0AF-5267B6942356}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Daniel S. Parra G.:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-107 instituciones inscritas más o menos el 40% ha comprado</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="EU21" authorId="0" shapeId="0" xr:uid="{0F47986C-FECA-4824-849A-6356BA883551}">
       <text>
         <r>
@@ -5611,31 +5564,6 @@
           </rPr>
           <t xml:space="preserve">
 No se hacen traslados</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="EI28" authorId="0" shapeId="0" xr:uid="{F027B743-5E2F-46C0-A27F-808C64B16BEA}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Daniel S. Parra G.:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-El 50% de las entidades inscritas (Dato pendiente)
-Este número se calculó acá</t>
         </r>
       </text>
     </comment>
@@ -7005,7 +6933,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3956" uniqueCount="1993">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3952" uniqueCount="1989">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -13118,9 +13046,6 @@
     <t>N0/C0</t>
   </si>
   <si>
-    <t>?612-445</t>
-  </si>
-  <si>
     <t>N2/C0</t>
   </si>
   <si>
@@ -13145,9 +13070,6 @@
     <t>N0/C2</t>
   </si>
   <si>
-    <t>?527--329</t>
-  </si>
-  <si>
     <t>N5/C0</t>
   </si>
   <si>
@@ -13169,13 +13091,7 @@
     <t>N0/C7</t>
   </si>
   <si>
-    <t>?163-433</t>
-  </si>
-  <si>
     <t>N0/C4</t>
-  </si>
-  <si>
-    <t>?281-266</t>
   </si>
   <si>
     <t>Meta</t>
@@ -13459,7 +13375,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -13496,6 +13412,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -13511,7 +13433,7 @@
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -13656,6 +13578,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13884,10 +13809,10 @@
   <dimension ref="A1:GH32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="FY2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomRight" activeCell="GG1" sqref="GG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14481,7 +14406,7 @@
         <v>44324.663341099542</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1976</v>
+        <v>1972</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>156</v>
@@ -14644,7 +14569,7 @@
         <v>192</v>
       </c>
       <c r="BY2" s="5" t="s">
-        <v>1933</v>
+        <v>1929</v>
       </c>
       <c r="CA2" s="2" t="s">
         <v>193</v>
@@ -14818,7 +14743,7 @@
       <c r="EH2" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="EI2" s="5">
+      <c r="EI2" s="32">
         <v>78</v>
       </c>
       <c r="EJ2" s="2" t="s">
@@ -14947,8 +14872,8 @@
       <c r="GE2" s="37" t="s">
         <v>1903</v>
       </c>
-      <c r="GF2" s="37" t="s">
-        <v>1904</v>
+      <c r="GF2" s="37">
+        <v>78</v>
       </c>
       <c r="GG2" s="33" t="s">
         <v>1887</v>
@@ -15094,7 +15019,7 @@
         <v>266</v>
       </c>
       <c r="BR3" s="2" t="s">
-        <v>1982</v>
+        <v>1978</v>
       </c>
       <c r="BT3" s="2" t="s">
         <v>267</v>
@@ -15112,10 +15037,10 @@
         <v>270</v>
       </c>
       <c r="BY3" s="5" t="s">
-        <v>1934</v>
+        <v>1930</v>
       </c>
       <c r="BZ3" s="5" t="s">
-        <v>1930</v>
+        <v>1926</v>
       </c>
       <c r="CA3" s="2" t="s">
         <v>216</v>
@@ -15276,7 +15201,7 @@
       <c r="EH3" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="EI3" s="2">
+      <c r="EI3" s="33">
         <v>300</v>
       </c>
       <c r="EJ3" s="2" t="s">
@@ -15397,13 +15322,13 @@
         <v>2</v>
       </c>
       <c r="GC3" s="37" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="GD3" s="59">
         <v>1</v>
       </c>
       <c r="GE3" s="37" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="GF3" s="37">
         <v>300</v>
@@ -15418,7 +15343,7 @@
         <v>44326.502545150463</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1976</v>
+        <v>1972</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>312</v>
@@ -15551,7 +15476,7 @@
         <v>334</v>
       </c>
       <c r="BR4" s="2" t="s">
-        <v>1982</v>
+        <v>1978</v>
       </c>
       <c r="BT4" s="2" t="s">
         <v>335</v>
@@ -15569,7 +15494,7 @@
         <v>337</v>
       </c>
       <c r="BY4" s="5" t="s">
-        <v>1938</v>
+        <v>1934</v>
       </c>
       <c r="CA4" s="2" t="s">
         <v>193</v>
@@ -15593,7 +15518,7 @@
         <v>196</v>
       </c>
       <c r="CH4" s="2" t="s">
-        <v>1978</v>
+        <v>1974</v>
       </c>
       <c r="CI4" s="2" t="s">
         <v>339</v>
@@ -15723,7 +15648,7 @@
         <v>193</v>
       </c>
       <c r="EB4" s="69" t="s">
-        <v>1992</v>
+        <v>1988</v>
       </c>
       <c r="ED4" s="2" t="s">
         <v>354</v>
@@ -15737,8 +15662,8 @@
       <c r="EH4" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="EI4" s="5">
-        <v>78</v>
+      <c r="EI4" s="32">
+        <v>1054</v>
       </c>
       <c r="EJ4" s="2" t="s">
         <v>357</v>
@@ -15822,7 +15747,7 @@
         <v>216</v>
       </c>
       <c r="FO4" s="24" t="s">
-        <v>1988</v>
+        <v>1984</v>
       </c>
       <c r="FP4" s="25">
         <v>12</v>
@@ -15858,16 +15783,16 @@
         <v>3</v>
       </c>
       <c r="GC4" s="37" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="GD4" s="67">
         <v>22</v>
       </c>
       <c r="GE4" s="38" t="s">
-        <v>1990</v>
+        <v>1986</v>
       </c>
       <c r="GF4" s="37">
-        <v>1054</v>
+        <v>78</v>
       </c>
       <c r="GG4" s="33" t="s">
         <v>1885</v>
@@ -16196,7 +16121,7 @@
       <c r="EH5" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="EI5" s="2">
+      <c r="EI5" s="33">
         <v>208</v>
       </c>
       <c r="EJ5" s="2" t="s">
@@ -16326,7 +16251,7 @@
         <v>2</v>
       </c>
       <c r="GC5" s="37" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="GD5" s="59">
         <v>0</v>
@@ -16346,7 +16271,7 @@
         <v>44339.650587766198</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1976</v>
+        <v>1972</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>440</v>
@@ -16494,7 +16419,7 @@
         <v>460</v>
       </c>
       <c r="BR6" s="2" t="s">
-        <v>1982</v>
+        <v>1978</v>
       </c>
       <c r="BT6" s="2" t="s">
         <v>461</v>
@@ -16668,7 +16593,7 @@
       <c r="EH6" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="EI6" s="2">
+      <c r="EI6" s="33">
         <v>103</v>
       </c>
       <c r="EJ6" s="2" t="s">
@@ -16792,7 +16717,7 @@
         <v>4</v>
       </c>
       <c r="GC6" s="37" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="GD6" s="59">
         <v>0</v>
@@ -16966,7 +16891,7 @@
         <v>515</v>
       </c>
       <c r="BR7" s="2" t="s">
-        <v>1983</v>
+        <v>1979</v>
       </c>
       <c r="BT7" s="2" t="s">
         <v>516</v>
@@ -16984,7 +16909,7 @@
         <v>518</v>
       </c>
       <c r="BY7" s="5" t="s">
-        <v>1935</v>
+        <v>1931</v>
       </c>
       <c r="CA7" s="2" t="s">
         <v>193</v>
@@ -17142,8 +17067,8 @@
       <c r="EH7" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="EI7" s="5" t="s">
-        <v>537</v>
+      <c r="EI7" s="32">
+        <v>358</v>
       </c>
       <c r="EJ7" s="2" t="s">
         <v>538</v>
@@ -17274,8 +17199,8 @@
       <c r="GE7" s="37" t="s">
         <v>1903</v>
       </c>
-      <c r="GF7" s="37">
-        <v>358</v>
+      <c r="GF7" s="37" t="s">
+        <v>537</v>
       </c>
       <c r="GG7" s="33" t="s">
         <v>1887</v>
@@ -17407,7 +17332,7 @@
         <v>571</v>
       </c>
       <c r="BR8" s="2" t="s">
-        <v>1984</v>
+        <v>1980</v>
       </c>
       <c r="BT8" s="2" t="s">
         <v>572</v>
@@ -17580,8 +17505,8 @@
       <c r="EH8" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="EI8" s="5" t="s">
-        <v>593</v>
+      <c r="EI8" s="32">
+        <v>176</v>
       </c>
       <c r="EJ8" s="2" t="s">
         <v>594</v>
@@ -17701,16 +17626,16 @@
         <v>1</v>
       </c>
       <c r="GC8" s="37" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="GD8" s="59">
         <v>1</v>
       </c>
       <c r="GE8" s="37" t="s">
-        <v>1906</v>
-      </c>
-      <c r="GF8" s="37">
-        <v>176</v>
+        <v>1905</v>
+      </c>
+      <c r="GF8" s="37" t="s">
+        <v>593</v>
       </c>
       <c r="GG8" s="33" t="s">
         <v>1889</v>
@@ -17908,7 +17833,7 @@
         <v>637</v>
       </c>
       <c r="BZ9" s="2" t="s">
-        <v>1932</v>
+        <v>1928</v>
       </c>
       <c r="CA9" s="2" t="s">
         <v>216</v>
@@ -18066,7 +17991,7 @@
       <c r="EH9" s="2" t="s">
         <v>654</v>
       </c>
-      <c r="EI9" s="2">
+      <c r="EI9" s="33">
         <v>34</v>
       </c>
       <c r="EJ9" s="2" t="s">
@@ -18187,13 +18112,13 @@
         <v>4</v>
       </c>
       <c r="GC9" s="37" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="GD9" s="59">
         <v>2</v>
       </c>
       <c r="GE9" s="37" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="GF9" s="37">
         <v>34</v>
@@ -18344,7 +18269,7 @@
         <v>688</v>
       </c>
       <c r="BR10" s="2" t="s">
-        <v>1984</v>
+        <v>1980</v>
       </c>
       <c r="BT10" s="2" t="s">
         <v>689</v>
@@ -18517,8 +18442,8 @@
       <c r="EH10" s="2" t="s">
         <v>708</v>
       </c>
-      <c r="EI10" s="5" t="s">
-        <v>709</v>
+      <c r="EI10" s="32">
+        <v>119</v>
       </c>
       <c r="EJ10" s="2" t="s">
         <v>710</v>
@@ -18641,16 +18566,16 @@
         <v>1</v>
       </c>
       <c r="GC10" s="37" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="GD10" s="59">
         <v>1</v>
       </c>
       <c r="GE10" s="37" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="GF10" s="37" t="s">
-        <v>1913</v>
+        <v>709</v>
       </c>
       <c r="GG10" s="33" t="s">
         <v>1890</v>
@@ -18977,7 +18902,7 @@
       <c r="EH11" s="2" t="s">
         <v>759</v>
       </c>
-      <c r="EI11" s="2">
+      <c r="EI11" s="33">
         <v>80</v>
       </c>
       <c r="EJ11" s="2" t="s">
@@ -19101,7 +19026,7 @@
         <v>5</v>
       </c>
       <c r="GC11" s="37" t="s">
-        <v>1914</v>
+        <v>1912</v>
       </c>
       <c r="GD11" s="59">
         <v>0</v>
@@ -19296,7 +19221,7 @@
         <v>800</v>
       </c>
       <c r="BY12" s="5" t="s">
-        <v>1939</v>
+        <v>1935</v>
       </c>
       <c r="CA12" s="2" t="s">
         <v>193</v>
@@ -19451,7 +19376,7 @@
       <c r="EH12" s="2" t="s">
         <v>813</v>
       </c>
-      <c r="EI12" s="2">
+      <c r="EI12" s="33">
         <v>245</v>
       </c>
       <c r="EJ12" s="2" t="s">
@@ -19575,13 +19500,13 @@
         <v>3</v>
       </c>
       <c r="GC12" s="37" t="s">
-        <v>1915</v>
+        <v>1913</v>
       </c>
       <c r="GD12" s="59">
         <v>8</v>
       </c>
       <c r="GE12" s="37" t="s">
-        <v>1916</v>
+        <v>1914</v>
       </c>
       <c r="GF12" s="37">
         <v>245</v>
@@ -19770,7 +19695,7 @@
         <v>855</v>
       </c>
       <c r="BY13" s="5" t="s">
-        <v>1936</v>
+        <v>1932</v>
       </c>
       <c r="CA13" s="2" t="s">
         <v>193</v>
@@ -19791,7 +19716,7 @@
         <v>274</v>
       </c>
       <c r="CH13" s="2" t="s">
-        <v>1979</v>
+        <v>1975</v>
       </c>
       <c r="CJ13" s="2" t="s">
         <v>801</v>
@@ -19926,8 +19851,8 @@
       <c r="EH13" s="2" t="s">
         <v>873</v>
       </c>
-      <c r="EI13" s="2">
-        <v>45</v>
+      <c r="EI13" s="33">
+        <v>570</v>
       </c>
       <c r="EJ13" s="2" t="s">
         <v>874</v>
@@ -20054,7 +19979,7 @@
         <v>6</v>
       </c>
       <c r="GC13" s="37" t="s">
-        <v>1917</v>
+        <v>1915</v>
       </c>
       <c r="GD13" s="59">
         <v>0</v>
@@ -20063,7 +19988,7 @@
         <v>1903</v>
       </c>
       <c r="GF13" s="36">
-        <v>570</v>
+        <v>45</v>
       </c>
       <c r="GG13" s="33" t="s">
         <v>1888</v>
@@ -20074,7 +19999,7 @@
         <v>44384.71444163195</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>1976</v>
+        <v>1972</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>905</v>
@@ -20203,7 +20128,7 @@
         <v>921</v>
       </c>
       <c r="BR14" s="1" t="s">
-        <v>1982</v>
+        <v>1978</v>
       </c>
       <c r="BT14" s="1" t="s">
         <v>922</v>
@@ -20239,7 +20164,7 @@
         <v>578</v>
       </c>
       <c r="CH14" s="1" t="s">
-        <v>1980</v>
+        <v>1976</v>
       </c>
       <c r="CJ14" s="1" t="s">
         <v>927</v>
@@ -20379,7 +20304,7 @@
       <c r="EH14" s="1" t="s">
         <v>941</v>
       </c>
-      <c r="EI14" s="1">
+      <c r="EI14" s="33">
         <v>43</v>
       </c>
       <c r="EJ14" s="1" t="s">
@@ -20503,7 +20428,7 @@
         <v>3</v>
       </c>
       <c r="GC14" s="58" t="s">
-        <v>1918</v>
+        <v>1916</v>
       </c>
       <c r="GD14" s="60">
         <v>0</v>
@@ -20652,7 +20577,7 @@
         <v>976</v>
       </c>
       <c r="BR15" s="1" t="s">
-        <v>1982</v>
+        <v>1978</v>
       </c>
       <c r="BT15" s="1" t="s">
         <v>977</v>
@@ -20825,7 +20750,7 @@
       <c r="EH15" s="1" t="s">
         <v>995</v>
       </c>
-      <c r="EI15" s="1">
+      <c r="EI15" s="33">
         <v>220</v>
       </c>
       <c r="EJ15" s="1" t="s">
@@ -20947,13 +20872,13 @@
         <v>2</v>
       </c>
       <c r="GC15" s="58" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="GD15" s="60">
         <v>6</v>
       </c>
       <c r="GE15" s="58" t="s">
-        <v>1919</v>
+        <v>1917</v>
       </c>
       <c r="GF15" s="58">
         <v>220</v>
@@ -21123,7 +21048,7 @@
         <v>1033</v>
       </c>
       <c r="BR16" s="1" t="s">
-        <v>1982</v>
+        <v>1978</v>
       </c>
       <c r="BT16" s="1" t="s">
         <v>1034</v>
@@ -21138,7 +21063,7 @@
         <v>1036</v>
       </c>
       <c r="BY16" s="15" t="s">
-        <v>1940</v>
+        <v>1936</v>
       </c>
       <c r="CA16" s="1" t="s">
         <v>193</v>
@@ -21295,7 +21220,7 @@
       <c r="EH16" s="1" t="s">
         <v>1050</v>
       </c>
-      <c r="EI16" s="1">
+      <c r="EI16" s="33">
         <v>130</v>
       </c>
       <c r="EJ16" s="1" t="s">
@@ -21422,7 +21347,7 @@
         <v>7</v>
       </c>
       <c r="GE16" s="58" t="s">
-        <v>1920</v>
+        <v>1918</v>
       </c>
       <c r="GF16" s="58">
         <v>130</v>
@@ -21436,7 +21361,7 @@
         <v>44447.520694444444</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>1976</v>
+        <v>1972</v>
       </c>
       <c r="C17" t="s">
         <v>1079</v>
@@ -21558,7 +21483,7 @@
         <v>1093</v>
       </c>
       <c r="BR17" t="s">
-        <v>1982</v>
+        <v>1978</v>
       </c>
       <c r="BT17" t="s">
         <v>1094</v>
@@ -21597,7 +21522,7 @@
         <v>274</v>
       </c>
       <c r="CH17" t="s">
-        <v>1980</v>
+        <v>1976</v>
       </c>
       <c r="CJ17" t="s">
         <v>1101</v>
@@ -21734,7 +21659,7 @@
       <c r="EH17" t="s">
         <v>1116</v>
       </c>
-      <c r="EI17">
+      <c r="EI17" s="37">
         <v>2</v>
       </c>
       <c r="EJ17" t="s">
@@ -21863,7 +21788,7 @@
         <v>1</v>
       </c>
       <c r="GC17" s="37" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="GD17" s="59">
         <v>0</v>
@@ -22192,7 +22117,7 @@
       <c r="EH18" t="s">
         <v>1162</v>
       </c>
-      <c r="EI18">
+      <c r="EI18" s="37">
         <v>78</v>
       </c>
       <c r="EJ18" t="s">
@@ -22316,7 +22241,7 @@
         <v>2</v>
       </c>
       <c r="GC18" s="37" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="GD18" s="59">
         <v>0</v>
@@ -22360,7 +22285,7 @@
         <v>773</v>
       </c>
       <c r="K19" s="24" t="s">
-        <v>1991</v>
+        <v>1987</v>
       </c>
       <c r="L19" s="68">
         <v>43128</v>
@@ -22450,7 +22375,7 @@
         <v>1185</v>
       </c>
       <c r="BR19" t="s">
-        <v>1982</v>
+        <v>1978</v>
       </c>
       <c r="BT19" t="s">
         <v>1186</v>
@@ -22486,7 +22411,7 @@
         <v>274</v>
       </c>
       <c r="CH19" t="s">
-        <v>1980</v>
+        <v>1976</v>
       </c>
       <c r="CJ19" t="s">
         <v>1191</v>
@@ -22620,7 +22545,7 @@
       <c r="EH19" t="s">
         <v>1204</v>
       </c>
-      <c r="EI19">
+      <c r="EI19" s="37">
         <v>11</v>
       </c>
       <c r="EJ19" s="21" t="s">
@@ -22738,13 +22663,13 @@
         <v>1</v>
       </c>
       <c r="GC19" s="37" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="GD19" s="59">
         <v>1</v>
       </c>
       <c r="GE19" s="37" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="GF19" s="37">
         <v>11</v>
@@ -22896,7 +22821,7 @@
         <v>1238</v>
       </c>
       <c r="BR20" t="s">
-        <v>1984</v>
+        <v>1980</v>
       </c>
       <c r="BT20" t="s">
         <v>1239</v>
@@ -22914,7 +22839,7 @@
         <v>1242</v>
       </c>
       <c r="BZ20" s="24" t="s">
-        <v>1931</v>
+        <v>1927</v>
       </c>
       <c r="CA20" t="s">
         <v>216</v>
@@ -22935,7 +22860,7 @@
         <v>578</v>
       </c>
       <c r="CH20" t="s">
-        <v>1981</v>
+        <v>1977</v>
       </c>
       <c r="CJ20" t="s">
         <v>1245</v>
@@ -23072,8 +22997,9 @@
       <c r="EH20" t="s">
         <v>1262</v>
       </c>
-      <c r="EI20" t="s">
-        <v>1249</v>
+      <c r="EI20" s="70">
+        <f>(433+163)/2</f>
+        <v>298</v>
       </c>
       <c r="EJ20" t="s">
         <v>1263</v>
@@ -23199,16 +23125,16 @@
         <v>1</v>
       </c>
       <c r="GC20" s="37" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="GD20" s="59">
         <v>1</v>
       </c>
       <c r="GE20" s="37" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="GF20" s="37" t="s">
-        <v>1921</v>
+        <v>1249</v>
       </c>
       <c r="GG20" s="33" t="s">
         <v>1888</v>
@@ -23396,7 +23322,7 @@
         <v>367</v>
       </c>
       <c r="CH21" t="s">
-        <v>1980</v>
+        <v>1976</v>
       </c>
       <c r="CJ21" t="s">
         <v>1307</v>
@@ -23527,8 +23453,7 @@
       <c r="EH21" t="s">
         <v>1317</v>
       </c>
-      <c r="EI21" s="25">
-        <f>ROUND(107*0.4,0)</f>
+      <c r="EI21" s="36">
         <v>43</v>
       </c>
       <c r="EJ21" t="s">
@@ -23672,7 +23597,7 @@
         <v>44430.608212476851</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>1976</v>
+        <v>1972</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>1335</v>
@@ -23834,7 +23759,7 @@
         <v>1353</v>
       </c>
       <c r="BR22" s="1" t="s">
-        <v>1982</v>
+        <v>1978</v>
       </c>
       <c r="BS22" s="13"/>
       <c r="BT22" s="1" t="s">
@@ -23876,7 +23801,7 @@
         <v>274</v>
       </c>
       <c r="CH22" s="1" t="s">
-        <v>1980</v>
+        <v>1976</v>
       </c>
       <c r="CI22" s="13"/>
       <c r="CJ22" s="1" t="s">
@@ -24022,7 +23947,7 @@
       <c r="EH22" s="1" t="s">
         <v>1373</v>
       </c>
-      <c r="EI22" s="1">
+      <c r="EI22" s="33">
         <v>55</v>
       </c>
       <c r="EJ22" s="1" t="s">
@@ -24147,7 +24072,7 @@
         <v>4</v>
       </c>
       <c r="GC22" s="37" t="s">
-        <v>1922</v>
+        <v>1919</v>
       </c>
       <c r="GD22" s="59">
         <v>0</v>
@@ -24503,7 +24428,7 @@
       <c r="EH23" s="1" t="s">
         <v>1420</v>
       </c>
-      <c r="EI23" s="1">
+      <c r="EI23" s="33">
         <v>6</v>
       </c>
       <c r="EJ23" s="1" t="s">
@@ -24630,13 +24555,13 @@
         <v>1</v>
       </c>
       <c r="GC23" s="37" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="GD23" s="59">
         <v>1</v>
       </c>
       <c r="GE23" s="37" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="GF23" s="37">
         <v>6</v>
@@ -24812,7 +24737,7 @@
         <v>1463</v>
       </c>
       <c r="BY24" s="24" t="s">
-        <v>1941</v>
+        <v>1937</v>
       </c>
       <c r="CA24" t="s">
         <v>216</v>
@@ -24845,7 +24770,7 @@
         <v>1467</v>
       </c>
       <c r="CM24" s="24" t="s">
-        <v>1929</v>
+        <v>1925</v>
       </c>
       <c r="CN24" t="s">
         <v>1468</v>
@@ -24973,8 +24898,8 @@
       <c r="EH24" s="29" t="s">
         <v>1481</v>
       </c>
-      <c r="EI24">
-        <v>146</v>
+      <c r="EI24" s="37">
+        <v>69</v>
       </c>
       <c r="EJ24" t="s">
         <v>1482</v>
@@ -25097,16 +25022,16 @@
         <v>1</v>
       </c>
       <c r="GC24" s="37" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="GD24" s="59">
         <v>2</v>
       </c>
       <c r="GE24" s="37" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="GF24" s="37">
-        <v>69</v>
+        <v>146</v>
       </c>
       <c r="GG24" s="33" t="s">
         <v>1887</v>
@@ -25117,7 +25042,7 @@
         <v>44325.680474537039</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>1976</v>
+        <v>1972</v>
       </c>
       <c r="C25" t="s">
         <v>1491</v>
@@ -25249,7 +25174,7 @@
         <v>1509</v>
       </c>
       <c r="BR25" s="22" t="s">
-        <v>1982</v>
+        <v>1978</v>
       </c>
       <c r="BT25" t="s">
         <v>1510</v>
@@ -25285,7 +25210,7 @@
         <v>274</v>
       </c>
       <c r="CH25" t="s">
-        <v>1980</v>
+        <v>1976</v>
       </c>
       <c r="CJ25" t="s">
         <v>1515</v>
@@ -25428,7 +25353,7 @@
       <c r="EH25" s="21" t="s">
         <v>1529</v>
       </c>
-      <c r="EI25">
+      <c r="EI25" s="37">
         <v>3</v>
       </c>
       <c r="EJ25" s="21" t="s">
@@ -25552,7 +25477,7 @@
         <v>2</v>
       </c>
       <c r="GC25" s="37" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="GD25" s="59">
         <v>0</v>
@@ -25707,7 +25632,7 @@
         <v>1560</v>
       </c>
       <c r="BR26" t="s">
-        <v>1985</v>
+        <v>1981</v>
       </c>
       <c r="BS26" t="s">
         <v>1561</v>
@@ -25889,8 +25814,8 @@
       <c r="EH26" t="s">
         <v>1579</v>
       </c>
-      <c r="EI26">
-        <v>13</v>
+      <c r="EI26" s="37">
+        <v>19</v>
       </c>
       <c r="EJ26" t="s">
         <v>1263</v>
@@ -26013,7 +25938,7 @@
         <v>3</v>
       </c>
       <c r="GC26" s="37" t="s">
-        <v>1915</v>
+        <v>1913</v>
       </c>
       <c r="GD26" s="59">
         <v>0</v>
@@ -26021,8 +25946,8 @@
       <c r="GE26" s="37" t="s">
         <v>1903</v>
       </c>
-      <c r="GF26" s="37" t="s">
-        <v>1923</v>
+      <c r="GF26" s="37">
+        <v>13</v>
       </c>
       <c r="GG26" s="33" t="s">
         <v>1888</v>
@@ -26174,7 +26099,7 @@
         <v>1621</v>
       </c>
       <c r="BR27" t="s">
-        <v>1982</v>
+        <v>1978</v>
       </c>
       <c r="BT27" t="s">
         <v>1622</v>
@@ -26192,7 +26117,7 @@
         <v>1624</v>
       </c>
       <c r="BY27" s="24" t="s">
-        <v>1935</v>
+        <v>1931</v>
       </c>
       <c r="CA27" t="s">
         <v>216</v>
@@ -26353,7 +26278,7 @@
       <c r="EH27" s="21" t="s">
         <v>1638</v>
       </c>
-      <c r="EI27">
+      <c r="EI27" s="37">
         <v>62</v>
       </c>
       <c r="EJ27" s="21" t="s">
@@ -26468,19 +26393,19 @@
         <v>1219</v>
       </c>
       <c r="GA27" t="s">
-        <v>1924</v>
+        <v>1920</v>
       </c>
       <c r="GB27" s="37">
         <v>3</v>
       </c>
       <c r="GC27" s="37" t="s">
-        <v>1915</v>
+        <v>1913</v>
       </c>
       <c r="GD27" s="59">
         <v>5</v>
       </c>
       <c r="GE27" s="37" t="s">
-        <v>1925</v>
+        <v>1921</v>
       </c>
       <c r="GF27" s="37">
         <v>62</v>
@@ -26617,7 +26542,7 @@
         <v>1669</v>
       </c>
       <c r="BR28" t="s">
-        <v>1983</v>
+        <v>1979</v>
       </c>
       <c r="BT28" t="s">
         <v>1670</v>
@@ -26793,7 +26718,7 @@
       <c r="EH28" t="s">
         <v>1687</v>
       </c>
-      <c r="EI28" s="5">
+      <c r="EI28" s="32">
         <v>336</v>
       </c>
       <c r="EJ28" t="s">
@@ -26917,13 +26842,13 @@
         <v>3</v>
       </c>
       <c r="GC28" s="37" t="s">
-        <v>1915</v>
+        <v>1913</v>
       </c>
       <c r="GD28" s="59">
         <v>5</v>
       </c>
       <c r="GE28" s="37" t="s">
-        <v>1926</v>
+        <v>1922</v>
       </c>
       <c r="GF28" s="37">
         <v>336</v>
@@ -27081,7 +27006,7 @@
         <v>1716</v>
       </c>
       <c r="BR29" s="22" t="s">
-        <v>1984</v>
+        <v>1980</v>
       </c>
       <c r="BT29" t="s">
         <v>1717</v>
@@ -27257,7 +27182,7 @@
       <c r="EH29" t="s">
         <v>1736</v>
       </c>
-      <c r="EI29">
+      <c r="EI29" s="37">
         <v>1</v>
       </c>
       <c r="EJ29" t="s">
@@ -27387,10 +27312,10 @@
         <v>2</v>
       </c>
       <c r="GE29" s="37" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="GF29" s="37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="GG29" s="33" t="s">
         <v>1899</v>
@@ -27401,7 +27326,7 @@
         <v>44456.611226851855</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>1976</v>
+        <v>1972</v>
       </c>
       <c r="C30" t="s">
         <v>1751</v>
@@ -27524,7 +27449,7 @@
         <v>1767</v>
       </c>
       <c r="BJ30" s="39" t="s">
-        <v>1977</v>
+        <v>1973</v>
       </c>
       <c r="BK30" t="s">
         <v>262</v>
@@ -27542,7 +27467,7 @@
         <v>1770</v>
       </c>
       <c r="BR30" t="s">
-        <v>1982</v>
+        <v>1978</v>
       </c>
       <c r="BT30" t="s">
         <v>1771</v>
@@ -27560,7 +27485,7 @@
         <v>1773</v>
       </c>
       <c r="BY30" s="24" t="s">
-        <v>1937</v>
+        <v>1933</v>
       </c>
       <c r="CA30" t="s">
         <v>193</v>
@@ -27723,7 +27648,7 @@
       <c r="EH30" s="39" t="s">
         <v>1835</v>
       </c>
-      <c r="EI30">
+      <c r="EI30" s="37">
         <v>224</v>
       </c>
       <c r="EJ30" s="39" t="s">
@@ -27845,7 +27770,7 @@
         <v>4</v>
       </c>
       <c r="GC30" s="37" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="GD30" s="59">
         <v>0</v>
@@ -28033,7 +27958,7 @@
         <v>1805</v>
       </c>
       <c r="BR31" s="22" t="s">
-        <v>1986</v>
+        <v>1982</v>
       </c>
       <c r="BS31" t="s">
         <v>1806</v>
@@ -28218,7 +28143,7 @@
       <c r="EH31" t="s">
         <v>1823</v>
       </c>
-      <c r="EI31">
+      <c r="EI31" s="37">
         <v>13</v>
       </c>
       <c r="EJ31" t="s">
@@ -28348,7 +28273,7 @@
         <v>5</v>
       </c>
       <c r="GE31" s="37" t="s">
-        <v>1925</v>
+        <v>1921</v>
       </c>
       <c r="GF31" s="37">
         <v>13</v>
@@ -28359,31 +28284,31 @@
     </row>
     <row r="32" spans="1:189" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>1948</v>
+        <v>1944</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>828</v>
       </c>
       <c r="C32" t="s">
-        <v>1942</v>
+        <v>1938</v>
       </c>
       <c r="D32" t="s">
-        <v>1943</v>
+        <v>1939</v>
       </c>
       <c r="E32" s="20">
         <v>44453</v>
       </c>
       <c r="F32" t="s">
-        <v>1927</v>
+        <v>1923</v>
       </c>
       <c r="G32" t="s">
-        <v>1928</v>
+        <v>1924</v>
       </c>
       <c r="H32" t="s">
-        <v>1944</v>
+        <v>1940</v>
       </c>
       <c r="I32" t="s">
-        <v>1945</v>
+        <v>1941</v>
       </c>
       <c r="J32">
         <v>3213945338</v>
@@ -28395,31 +28320,31 @@
         <v>773</v>
       </c>
       <c r="M32" t="s">
-        <v>1946</v>
+        <v>1942</v>
       </c>
       <c r="N32" t="s">
-        <v>1947</v>
+        <v>1943</v>
       </c>
       <c r="O32" t="s">
-        <v>1942</v>
+        <v>1938</v>
       </c>
       <c r="P32" t="s">
         <v>166</v>
       </c>
       <c r="Q32" s="24" t="s">
-        <v>1987</v>
+        <v>1983</v>
       </c>
       <c r="R32" t="s">
         <v>168</v>
       </c>
       <c r="T32" t="s">
-        <v>1949</v>
+        <v>1945</v>
       </c>
       <c r="U32" t="s">
         <v>166</v>
       </c>
       <c r="V32" t="s">
-        <v>1950</v>
+        <v>1946</v>
       </c>
       <c r="W32" t="s">
         <v>171</v>
@@ -28449,7 +28374,7 @@
         <v>1100</v>
       </c>
       <c r="AZ32" t="s">
-        <v>1951</v>
+        <v>1947</v>
       </c>
       <c r="BA32" t="s">
         <v>175</v>
@@ -28458,43 +28383,43 @@
         <v>256</v>
       </c>
       <c r="BE32" t="s">
-        <v>1952</v>
+        <v>1948</v>
       </c>
       <c r="BF32" t="s">
-        <v>1953</v>
+        <v>1949</v>
       </c>
       <c r="BG32">
         <v>60</v>
       </c>
       <c r="BH32" t="s">
-        <v>1954</v>
+        <v>1950</v>
       </c>
       <c r="BI32" t="s">
         <v>511</v>
       </c>
       <c r="BJ32" t="s">
-        <v>1955</v>
+        <v>1951</v>
       </c>
       <c r="BK32" t="s">
         <v>262</v>
       </c>
       <c r="BM32" t="s">
-        <v>1956</v>
+        <v>1952</v>
       </c>
       <c r="BO32" t="s">
-        <v>1957</v>
+        <v>1953</v>
       </c>
       <c r="BP32" t="s">
         <v>187</v>
       </c>
       <c r="BQ32" t="s">
-        <v>1958</v>
+        <v>1954</v>
       </c>
       <c r="BR32" s="22" t="s">
-        <v>1984</v>
+        <v>1980</v>
       </c>
       <c r="BT32" t="s">
-        <v>1959</v>
+        <v>1955</v>
       </c>
       <c r="BU32" t="s">
         <v>380</v>
@@ -28506,10 +28431,10 @@
         <v>1157</v>
       </c>
       <c r="BX32" t="s">
-        <v>1960</v>
+        <v>1956</v>
       </c>
       <c r="BY32" t="s">
-        <v>1961</v>
+        <v>1957</v>
       </c>
       <c r="CA32" t="s">
         <v>193</v>
@@ -28518,13 +28443,13 @@
         <v>268</v>
       </c>
       <c r="CC32" s="22" t="s">
-        <v>1962</v>
+        <v>1958</v>
       </c>
       <c r="CD32" t="s">
         <v>856</v>
       </c>
       <c r="CE32" t="s">
-        <v>1963</v>
+        <v>1959</v>
       </c>
       <c r="CF32" t="s">
         <v>547</v>
@@ -28569,7 +28494,7 @@
         <v>281</v>
       </c>
       <c r="CX32" s="21" t="s">
-        <v>1964</v>
+        <v>1960</v>
       </c>
       <c r="CY32" t="s">
         <v>1192</v>
@@ -28596,10 +28521,10 @@
         <v>283</v>
       </c>
       <c r="DG32" t="s">
-        <v>1965</v>
+        <v>1961</v>
       </c>
       <c r="DH32" t="s">
-        <v>1966</v>
+        <v>1962</v>
       </c>
       <c r="DI32" s="22" t="s">
         <v>773</v>
@@ -28629,7 +28554,7 @@
         <v>208</v>
       </c>
       <c r="DU32" t="s">
-        <v>1967</v>
+        <v>1963</v>
       </c>
       <c r="DV32" t="s">
         <v>380</v>
@@ -28650,7 +28575,7 @@
         <v>756</v>
       </c>
       <c r="ED32" t="s">
-        <v>1968</v>
+        <v>1964</v>
       </c>
       <c r="EE32" t="s">
         <v>193</v>
@@ -28659,12 +28584,12 @@
         <v>222</v>
       </c>
       <c r="EG32" s="24" t="s">
-        <v>1989</v>
+        <v>1985</v>
       </c>
       <c r="EH32" t="s">
-        <v>1969</v>
-      </c>
-      <c r="EI32">
+        <v>1965</v>
+      </c>
+      <c r="EI32" s="37">
         <v>1</v>
       </c>
       <c r="EJ32" t="s">
@@ -28674,7 +28599,7 @@
         <v>773</v>
       </c>
       <c r="EL32" t="s">
-        <v>1970</v>
+        <v>1966</v>
       </c>
       <c r="EM32" t="s">
         <v>1157</v>
@@ -28692,13 +28617,13 @@
         <v>1157</v>
       </c>
       <c r="ES32" t="s">
-        <v>1971</v>
+        <v>1967</v>
       </c>
       <c r="ET32" t="s">
         <v>236</v>
       </c>
       <c r="EU32" t="s">
-        <v>1972</v>
+        <v>1968</v>
       </c>
       <c r="EV32" t="s">
         <v>1059</v>
@@ -28713,10 +28638,10 @@
         <v>236</v>
       </c>
       <c r="FA32" t="s">
-        <v>1973</v>
+        <v>1969</v>
       </c>
       <c r="FB32" t="s">
-        <v>1974</v>
+        <v>1970</v>
       </c>
       <c r="FC32" t="s">
         <v>274</v>
@@ -28725,7 +28650,7 @@
         <v>491</v>
       </c>
       <c r="FE32" t="s">
-        <v>1975</v>
+        <v>1971</v>
       </c>
       <c r="FF32" t="s">
         <v>434</v>
@@ -28776,19 +28701,19 @@
         <v>1078</v>
       </c>
       <c r="GA32" t="s">
-        <v>1927</v>
+        <v>1923</v>
       </c>
       <c r="GB32" s="37">
         <v>2</v>
       </c>
       <c r="GC32" s="37" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="GD32" s="59">
         <v>1</v>
       </c>
       <c r="GE32" s="37" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="GF32" s="37">
         <v>1</v>

</xml_diff>

<commit_message>
Reorganización y consolidación de capítulos de recetarios
</commit_message>
<xml_diff>
--- a/data/intermediate/001_Herramienta_Limpieza_Manual.xlsx
+++ b/data/intermediate/001_Herramienta_Limpieza_Manual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\OneDrive\Documents\Trabajos\UAS-FNE-2\61_Regionalizacion\FRE_AnalisisEstadistico\data\intermediate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E9AEC0-724A-4E9F-8066-AB1118D79931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8DE6A0-49CA-4E59-8C38-9578937BC374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -207,6 +207,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="DI2" authorId="0" shapeId="0" xr:uid="{863D1D3F-2FB8-4AD8-A51C-DC8BDD013D41}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Daniel S. Parra G.:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+4 horas</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="DK2" authorId="0" shapeId="0" xr:uid="{371786DF-91E3-47C9-B954-B31E1FF18BEC}">
       <text>
         <r>
@@ -2985,7 +3009,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Depende de la cantidad</t>
+Depende de la cantidad
+Decía que NA</t>
         </r>
       </text>
     </comment>
@@ -7105,7 +7130,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-No se hace</t>
+No se hace
+Se le pone que 1 ya que se esperan tamaños de pedidos pequeños</t>
         </r>
       </text>
     </comment>
@@ -7197,7 +7223,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3948" uniqueCount="1980">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3948" uniqueCount="1982">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -13541,6 +13567,18 @@
   </si>
   <si>
     <t>Microletras / microtexto, Sellos/Escudos, Codificación</t>
+  </si>
+  <si>
+    <t>- llega el pedido por parte de La empresa transportadora
+- La regente en farmacia La recepciona en el área de recepción técnica y administrativa
+- Se contrasta con La guía
+- Observación de condiciones
+- almacenamiento de los productos</t>
+  </si>
+  <si>
+    <t>- Se hace La comparación de los productos allegados contra La orden de compra
+- Se realiza inspección física y técnica del material
+- Se disponen los productos para su correspondiente almacenamiento</t>
   </si>
 </sst>
 </file>
@@ -14047,10 +14085,10 @@
   <dimension ref="A1:GH32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="BW2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="BP2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BY1" sqref="BY1"/>
+      <selection pane="bottomRight" activeCell="BQ1" sqref="BQ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14908,8 +14946,8 @@
       <c r="DH2" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="DI2" s="2">
-        <v>4</v>
+      <c r="DI2" s="5">
+        <v>1</v>
       </c>
       <c r="DJ2" s="2" t="s">
         <v>211</v>
@@ -20023,8 +20061,8 @@
       <c r="DH13" s="2" t="s">
         <v>862</v>
       </c>
-      <c r="DI13" s="5" t="s">
-        <v>771</v>
+      <c r="DI13" s="5">
+        <v>1</v>
       </c>
       <c r="DJ13" s="2" t="s">
         <v>863</v>
@@ -21826,11 +21864,8 @@
       <c r="DG17" t="s">
         <v>1103</v>
       </c>
-      <c r="DH17" t="e" cm="1">
-        <f t="array" ref="DH17">- Se hace La comparación de los productos allegados contra La orden de compra
-- Se realiza inspección física y técnica del material
-- Se disponen los productos para su correspondiente almacenamiento</f>
-        <v>#NAME?</v>
+      <c r="DH17" s="39" t="s">
+        <v>1981</v>
       </c>
       <c r="DI17">
         <v>1</v>
@@ -27808,13 +27843,8 @@
       <c r="DG30" t="s">
         <v>1768</v>
       </c>
-      <c r="DH30" t="e" cm="1">
-        <f t="array" ref="DH30">- llega el pedido por parte de La empresa transportadora
-- La regente en farmacia La recepciona en el área de recepción técnica y administrativa
-- Se contrasta con La guía
-- Observación de condiciones
-- almacenamiento de los productos</f>
-        <v>#NAME?</v>
+      <c r="DH30" s="39" t="s">
+        <v>1980</v>
       </c>
       <c r="DI30">
         <v>1</v>
@@ -28757,8 +28787,8 @@
       <c r="DH32" t="s">
         <v>1951</v>
       </c>
-      <c r="DI32" s="22" t="s">
-        <v>771</v>
+      <c r="DI32" s="22">
+        <v>1</v>
       </c>
       <c r="DJ32" s="22" t="s">
         <v>771</v>

</xml_diff>

<commit_message>
Actualización y reforma de Capítulo de MME
</commit_message>
<xml_diff>
--- a/data/intermediate/001_Herramienta_Limpieza_Manual.xlsx
+++ b/data/intermediate/001_Herramienta_Limpieza_Manual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\OneDrive\Documents\Trabajos\UAS-FNE-2\61_Regionalizacion\FRE_AnalisisEstadistico\data\intermediate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE2CC8D-0C31-4838-A895-9C0E98D8B779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EADC2C-E22E-4FE9-AD2A-60D1384AE96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14106,10 +14106,10 @@
   <dimension ref="A1:GH32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="DQ2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="FN2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DU25" sqref="DU25"/>
+      <selection pane="bottomRight" activeCell="FN1" sqref="FN1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -29005,7 +29005,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:GG32" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
Se adicionan grafico 3D de clasificación a informe, se cambiand tos de Antioquia, se arregla responsividad en móviles
</commit_message>
<xml_diff>
--- a/data/intermediate/001_Herramienta_Limpieza_Manual.xlsx
+++ b/data/intermediate/001_Herramienta_Limpieza_Manual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\OneDrive\Documents\Trabajos\UAS-FNE-2\61_Regionalizacion\FRE_AnalisisEstadistico\data\intermediate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EADC2C-E22E-4FE9-AD2A-60D1384AE96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DEDF67-2338-4DB1-9BF1-75DA4646804F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -684,7 +684,32 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-9568 decía</t>
+9568 decía
+77 decía</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AT4" authorId="0" shapeId="0" xr:uid="{FEB882E7-1C2D-4291-B5ED-FE946A118D27}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Daniel S. Parra G.:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+25 semanas decía</t>
         </r>
       </text>
     </comment>
@@ -14106,10 +14131,10 @@
   <dimension ref="A1:GH32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="FN2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="AP2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="FN1" sqref="FN1"/>
+      <selection pane="bottomRight" activeCell="AS1" sqref="AS1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -15703,13 +15728,14 @@
         <v>171</v>
       </c>
       <c r="AR4" s="5">
-        <v>77</v>
+        <v>25000</v>
       </c>
       <c r="AS4" s="5" t="s">
         <v>882</v>
       </c>
-      <c r="AT4" s="2">
-        <v>25</v>
+      <c r="AT4" s="5">
+        <f>52*2</f>
+        <v>104</v>
       </c>
       <c r="AU4" s="2">
         <v>3</v>

</xml_diff>

<commit_message>
Cambios en gráficos del proyecto
</commit_message>
<xml_diff>
--- a/data/intermediate/001_Herramienta_Limpieza_Manual.xlsx
+++ b/data/intermediate/001_Herramienta_Limpieza_Manual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\OneDrive\Documents\Trabajos\UAS-FNE-2\61_Regionalizacion\FRE_AnalisisEstadistico\data\intermediate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DEDF67-2338-4DB1-9BF1-75DA4646804F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68BFA3B-9A6F-4CB0-A8DA-0CDBD17E5FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7272,7 +7272,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3948" uniqueCount="1981">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3950" uniqueCount="1983">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -13625,6 +13625,12 @@
   </si>
   <si>
     <t>Insuficientes para el FRE</t>
+  </si>
+  <si>
+    <t>Act_Impr</t>
+  </si>
+  <si>
+    <t>Act_Impr_2</t>
   </si>
 </sst>
 </file>
@@ -14128,13 +14134,13 @@
   <sheetPr codeName="Hoja1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:GH32"/>
+  <dimension ref="A1:GI32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="AP2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="GA2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AS1" sqref="AS1"/>
+      <selection pane="bottomRight" activeCell="GI1" sqref="GI1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14154,7 +14160,7 @@
     <col min="188" max="188" width="21.5703125" style="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14722,8 +14728,14 @@
       <c r="GG1" s="33" t="s">
         <v>1893</v>
       </c>
+      <c r="GH1" t="s">
+        <v>1981</v>
+      </c>
+      <c r="GI1" t="s">
+        <v>1982</v>
+      </c>
     </row>
-    <row r="2" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>44324.663341099542</v>
       </c>
@@ -14841,7 +14853,7 @@
       <c r="BF2" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="BG2" s="2">
+      <c r="BG2" s="5">
         <f>(30+15)</f>
         <v>45</v>
       </c>
@@ -15200,8 +15212,14 @@
       <c r="GG2" s="33" t="s">
         <v>1879</v>
       </c>
+      <c r="GH2">
+        <v>17</v>
+      </c>
+      <c r="GI2">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>44326.360274907405</v>
       </c>
@@ -15658,9 +15676,14 @@
       <c r="GG3" s="33" t="s">
         <v>1878</v>
       </c>
-      <c r="GH3" s="22"/>
+      <c r="GH3" s="22">
+        <v>173</v>
+      </c>
+      <c r="GI3">
+        <v>56</v>
+      </c>
     </row>
-    <row r="4" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>44326.502545150463</v>
       </c>
@@ -16120,8 +16143,14 @@
       <c r="GG4" s="33" t="s">
         <v>1877</v>
       </c>
+      <c r="GH4">
+        <v>559</v>
+      </c>
+      <c r="GI4">
+        <v>234</v>
+      </c>
     </row>
-    <row r="5" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>44337.64144068287</v>
       </c>
@@ -16588,8 +16617,14 @@
       <c r="GG5" s="33" t="s">
         <v>1879</v>
       </c>
+      <c r="GH5">
+        <v>10</v>
+      </c>
+      <c r="GI5">
+        <v>6</v>
+      </c>
     </row>
-    <row r="6" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>44339.650587766198</v>
       </c>
@@ -17054,8 +17089,14 @@
       <c r="GG6" s="33" t="s">
         <v>1880</v>
       </c>
+      <c r="GH6">
+        <v>46</v>
+      </c>
+      <c r="GI6">
+        <v>29</v>
+      </c>
     </row>
-    <row r="7" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>44341.914503842592</v>
       </c>
@@ -17528,8 +17569,14 @@
       <c r="GG7" s="33" t="s">
         <v>1879</v>
       </c>
+      <c r="GH7">
+        <v>21</v>
+      </c>
+      <c r="GI7">
+        <v>9</v>
+      </c>
     </row>
-    <row r="8" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>44342.470375613426</v>
       </c>
@@ -17963,8 +18010,14 @@
       <c r="GG8" s="33" t="s">
         <v>1881</v>
       </c>
+      <c r="GH8">
+        <v>13</v>
+      </c>
+      <c r="GI8">
+        <v>7</v>
+      </c>
     </row>
-    <row r="9" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>44342.499626712961</v>
       </c>
@@ -18447,8 +18500,14 @@
       <c r="GG9" s="33" t="s">
         <v>1878</v>
       </c>
+      <c r="GH9">
+        <v>18</v>
+      </c>
+      <c r="GI9">
+        <v>5</v>
+      </c>
     </row>
-    <row r="10" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>44342.542538240741</v>
       </c>
@@ -18901,8 +18960,14 @@
       <c r="GG10" s="33" t="s">
         <v>1882</v>
       </c>
+      <c r="GH10">
+        <v>9</v>
+      </c>
+      <c r="GI10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="11" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>44344.505199409723</v>
       </c>
@@ -19361,8 +19426,14 @@
       <c r="GG11" s="33" t="s">
         <v>1878</v>
       </c>
+      <c r="GH11">
+        <v>12</v>
+      </c>
+      <c r="GI11">
+        <v>3</v>
+      </c>
     </row>
-    <row r="12" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>44344.528835266203</v>
       </c>
@@ -19835,8 +19906,14 @@
       <c r="GG12" s="33" t="s">
         <v>1883</v>
       </c>
+      <c r="GH12">
+        <v>21</v>
+      </c>
+      <c r="GI12">
+        <v>8</v>
+      </c>
     </row>
-    <row r="13" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>44345.273268472221</v>
       </c>
@@ -20314,8 +20391,14 @@
       <c r="GG13" s="33" t="s">
         <v>1880</v>
       </c>
+      <c r="GH13">
+        <v>384</v>
+      </c>
+      <c r="GI13">
+        <v>158</v>
+      </c>
     </row>
-    <row r="14" spans="1:190" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:191" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12">
         <v>44384.71444163195</v>
       </c>
@@ -20763,8 +20846,14 @@
       <c r="GG14" s="33" t="s">
         <v>1884</v>
       </c>
+      <c r="GH14" s="13">
+        <v>1</v>
+      </c>
+      <c r="GI14" s="13">
+        <v>2</v>
+      </c>
     </row>
-    <row r="15" spans="1:190" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:191" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12">
         <v>44385.476659016203</v>
       </c>
@@ -21207,8 +21296,14 @@
       <c r="GG15" s="33" t="s">
         <v>1879</v>
       </c>
+      <c r="GH15" s="13">
+        <v>19</v>
+      </c>
+      <c r="GI15" s="13">
+        <v>7</v>
+      </c>
     </row>
-    <row r="16" spans="1:190" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:191" s="13" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12">
         <v>44385.485729236112</v>
       </c>
@@ -21676,8 +21771,14 @@
       <c r="GG16" s="33" t="s">
         <v>1885</v>
       </c>
+      <c r="GH16" s="13">
+        <v>19</v>
+      </c>
+      <c r="GI16" s="13">
+        <v>4</v>
+      </c>
     </row>
-    <row r="17" spans="1:189" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20">
         <v>44447.520694444444</v>
       </c>
@@ -22120,8 +22221,14 @@
       <c r="GG17" s="33" t="s">
         <v>1886</v>
       </c>
+      <c r="GH17">
+        <v>0</v>
+      </c>
+      <c r="GI17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:189" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20">
         <v>44508.834780092591</v>
       </c>
@@ -22573,8 +22680,14 @@
       <c r="GG18" s="33" t="s">
         <v>1879</v>
       </c>
+      <c r="GH18">
+        <v>9</v>
+      </c>
+      <c r="GI18">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="1:189" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="20">
         <v>44538.361712962964</v>
       </c>
@@ -22995,8 +23108,14 @@
       <c r="GG19" s="33" t="s">
         <v>1887</v>
       </c>
+      <c r="GH19">
+        <v>3</v>
+      </c>
+      <c r="GI19">
+        <v>1</v>
+      </c>
     </row>
-    <row r="20" spans="1:189" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20">
         <v>44538.366678240738</v>
       </c>
@@ -23457,8 +23576,14 @@
       <c r="GG20" s="33" t="s">
         <v>1880</v>
       </c>
+      <c r="GH20">
+        <v>17</v>
+      </c>
+      <c r="GI20">
+        <v>6</v>
+      </c>
     </row>
-    <row r="21" spans="1:189" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="20">
         <v>44538.47859953704</v>
       </c>
@@ -23909,8 +24034,14 @@
       <c r="GG21" s="33" t="s">
         <v>1879</v>
       </c>
+      <c r="GH21">
+        <v>4</v>
+      </c>
+      <c r="GI21">
+        <v>3</v>
+      </c>
     </row>
-    <row r="22" spans="1:189" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12">
         <v>44430.608212476851</v>
       </c>
@@ -24404,8 +24535,14 @@
       <c r="GG22" s="33" t="s">
         <v>1888</v>
       </c>
+      <c r="GH22">
+        <v>1</v>
+      </c>
+      <c r="GI22">
+        <v>3</v>
+      </c>
     </row>
-    <row r="23" spans="1:189" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12">
         <v>44437.434295497689</v>
       </c>
@@ -24887,8 +25024,14 @@
       <c r="GG23" s="33" t="s">
         <v>1889</v>
       </c>
+      <c r="GH23">
+        <v>0</v>
+      </c>
+      <c r="GI23">
+        <v>1</v>
+      </c>
     </row>
-    <row r="24" spans="1:189" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="20">
         <v>44438.904224537036</v>
       </c>
@@ -25354,8 +25497,14 @@
       <c r="GG24" s="33" t="s">
         <v>1879</v>
       </c>
+      <c r="GH24">
+        <v>44</v>
+      </c>
+      <c r="GI24">
+        <v>13</v>
+      </c>
     </row>
-    <row r="25" spans="1:189" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="20">
         <v>44325.680474537039</v>
       </c>
@@ -25809,8 +25958,14 @@
       <c r="GG25" s="33" t="s">
         <v>1890</v>
       </c>
+      <c r="GH25">
+        <v>0</v>
+      </c>
+      <c r="GI25">
+        <v>2</v>
+      </c>
     </row>
-    <row r="26" spans="1:189" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="20">
         <v>44386.04614583333</v>
       </c>
@@ -26268,8 +26423,14 @@
       <c r="GG26" s="33" t="s">
         <v>1880</v>
       </c>
+      <c r="GH26">
+        <v>5</v>
+      </c>
+      <c r="GI26">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:189" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="20">
         <v>44417.745393518519</v>
       </c>
@@ -26729,8 +26890,14 @@
       <c r="GG27" s="33" t="s">
         <v>1878</v>
       </c>
+      <c r="GH27">
+        <v>20</v>
+      </c>
+      <c r="GI27">
+        <v>13</v>
+      </c>
     </row>
-    <row r="28" spans="1:189" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="20">
         <v>44539.722870370373</v>
       </c>
@@ -27172,8 +27339,14 @@
       <c r="GG28" s="33" t="s">
         <v>1879</v>
       </c>
+      <c r="GH28">
+        <v>82</v>
+      </c>
+      <c r="GI28">
+        <v>31</v>
+      </c>
     </row>
-    <row r="29" spans="1:189" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="20">
         <v>44452.834814814814</v>
       </c>
@@ -27636,8 +27809,14 @@
       <c r="GG29" s="33" t="s">
         <v>1891</v>
       </c>
+      <c r="GH29">
+        <v>2</v>
+      </c>
+      <c r="GI29">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:189" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="20">
         <v>44456.611226851855</v>
       </c>
@@ -28095,8 +28274,14 @@
       <c r="GG30" s="33" t="s">
         <v>1879</v>
       </c>
+      <c r="GH30">
+        <v>19</v>
+      </c>
+      <c r="GI30">
+        <v>11</v>
+      </c>
     </row>
-    <row r="31" spans="1:189" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="20">
         <v>44458.952546296299</v>
       </c>
@@ -28589,8 +28774,14 @@
       <c r="GG31" s="33" t="s">
         <v>1892</v>
       </c>
+      <c r="GH31">
+        <v>1</v>
+      </c>
+      <c r="GI31">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:189" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="71">
         <v>44459.652824074074</v>
       </c>
@@ -29028,6 +29219,12 @@
       </c>
       <c r="GG32" s="33" t="s">
         <v>1878</v>
+      </c>
+      <c r="GH32">
+        <v>0</v>
+      </c>
+      <c r="GI32">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>